<commit_message>
fixing the names of the nav links ids this fixes #24 and reverts commit 58c8f7f
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\13IA\Project\13IA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="8_{6C6B00ED-0001-4830-AFB3-FBB4E517560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AAB373D-B2A7-4981-B118-868791D063C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2670" windowWidth="29040" windowHeight="15840" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <r>
       <t>&lt;</t>
@@ -2782,6 +2782,24 @@
   </si>
   <si>
     <t>for issues and dev</t>
+  </si>
+  <si>
+    <t>Back End</t>
+  </si>
+  <si>
+    <t>auto updates</t>
+  </si>
+  <si>
+    <t>calculations</t>
+  </si>
+  <si>
+    <t>data entry</t>
+  </si>
+  <si>
+    <t>data base</t>
+  </si>
+  <si>
+    <t>web server</t>
   </si>
 </sst>
 </file>
@@ -2867,10 +2885,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3170,58 +3184,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD87F2E1-A52F-4456-AB4D-EECF95DE5FBF}">
-  <dimension ref="B5:G82"/>
+  <dimension ref="B4:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E12:E29"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3229,7 +3264,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
@@ -3237,7 +3272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -3245,7 +3280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -3253,12 +3288,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
adding data to the history table
Signed-off-by: YelloElefant <alextrotternz@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\13IA\Project\13IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F19FDBB1-E2BD-4B39-96FE-3D4605BB12B4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
+    <workbookView minimized="1" xWindow="-18000" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
   <si>
     <r>
       <t>&lt;</t>
@@ -2715,9 +2737,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>public view test</t>
-  </si>
-  <si>
     <t xml:space="preserve">project management </t>
   </si>
   <si>
@@ -2793,20 +2812,260 @@
     <t>calculations</t>
   </si>
   <si>
-    <t>data entry</t>
-  </si>
-  <si>
     <t>data base</t>
   </si>
   <si>
     <t>web server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christchurch 1985 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 14-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Auckland Grammar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napier 1986 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 8-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Napier BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland 1987 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 12-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellington 1988 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 17-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. St Stephen’s School </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunedin 1989 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 6-4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton 1990 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 12-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christchurch 1991 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 18-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napier 1992 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 9-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mt Albert Grammar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland 1993 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 20-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellington 1994 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 26-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunedin 1995 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 9-5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton 1996 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 22-5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christchurch 1997 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 16-13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napier 1998 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 14-13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland 1999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 13-12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Otago BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellington 2000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 18-7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hastings BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunedin 2001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 27-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Auckland Grammar School </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palmerston North 2002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napier 2003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 22-14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton 2004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 47-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christchurch 2005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 20-12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Christchurch BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tauranga 2006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 15-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Wellington College </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wesley 2007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 18-15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Palmerston North BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellington 2008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 20-3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Plymouth 2009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 24-5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Bede’s 2010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 14-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hastings 2011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 10-7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Tauranga Boys’ College </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotorua 2012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 38-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auckland 2013 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 14-7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hamilton BHS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palmerston North 2014 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 27-26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunedin 2015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Wesley College </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massey High School 2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Auckland Grammar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellington 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final 22-18 </t>
+  </si>
+  <si>
+    <t>Auckland Grammar 2018</t>
+  </si>
+  <si>
+    <t>Final 17-21</t>
+  </si>
+  <si>
+    <t>1. Hamilton BHS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2840,6 +3099,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2849,10 +3121,54 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2861,7 +3177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2870,6 +3186,37 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3184,477 +3531,2254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD87F2E1-A52F-4456-AB4D-EECF95DE5FBF}">
-  <dimension ref="B4:I82"/>
+  <dimension ref="B3:Q197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L107" sqref="L6:L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I4" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1985 &lt;/td&gt;</v>
+      </c>
+      <c r="L6" t="str" cm="1">
+        <f t="array" ref="L6">INDEX(K$6:K$107,ROWS(K6:K$107))</f>
+        <v>&lt;td&gt;1. Hamilton BHS&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="K7" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O5, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L7" t="str" cm="1">
+        <f t="array" ref="L7">INDEX(K$6:K$107,ROWS(K7:K$107))</f>
+        <v>&lt;td&gt;Final 17-21&lt;/td&gt;</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L8" t="str" cm="1">
+        <f t="array" ref="L8">INDEX(K$6:K$107,ROWS(K8:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland Grammar 2018&lt;/td&gt;</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1986 &lt;/td&gt;</v>
+      </c>
+      <c r="L9" t="str" cm="1">
+        <f t="array" ref="L9">INDEX(K$6:K$107,ROWS(K9:K$107))</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P5, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 8-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L10" t="str" cm="1">
+        <f t="array" ref="L10">INDEX(K$6:K$107,ROWS(K10:K$107))</f>
+        <v>&lt;td&gt;Final 22-18 &lt;/td&gt;</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L11" t="str" cm="1">
+        <f t="array" ref="L11">INDEX(K$6:K$107,ROWS(K11:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2017 &lt;/td&gt;</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>9</v>
+      <c r="K12" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
+      </c>
+      <c r="L12" t="str" cm="1">
+        <f t="array" ref="L12">INDEX(K$6:K$107,ROWS(K12:K$107))</f>
+        <v>&lt;td&gt;1.Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="K13" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q5, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 12-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L13" t="str" cm="1">
+        <f t="array" ref="L13">INDEX(K$6:K$107,ROWS(K13:K$107))</f>
+        <v>&lt;td&gt;Final &lt;/td&gt;</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L14" t="str" cm="1">
+        <f t="array" ref="L14">INDEX(K$6:K$107,ROWS(K14:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Massey High School 2016 &lt;/td&gt;</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>
+      </c>
+      <c r="L15" t="str" cm="1">
+        <f t="array" ref="L15">INDEX(K$6:K$107,ROWS(K15:K$107))</f>
+        <v>&lt;td&gt;1.Wesley College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O8, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 17-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L16" t="str" cm="1">
+        <f t="array" ref="L16">INDEX(K$6:K$107,ROWS(K16:K$107))</f>
+        <v>&lt;td&gt;Final &lt;/td&gt;</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L17" t="str" cm="1">
+        <f t="array" ref="L17">INDEX(K$6:K$107,ROWS(K17:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2015 &lt;/td&gt;</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
+      </c>
+      <c r="L18" t="str" cm="1">
+        <f t="array" ref="L18">INDEX(K$6:K$107,ROWS(K18:K$107))</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P8, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 6-4 &lt;/td&gt;</v>
+      </c>
+      <c r="L19" t="str" cm="1">
+        <f t="array" ref="L19">INDEX(K$6:K$107,ROWS(K19:K$107))</f>
+        <v>&lt;td&gt;Final 27-26 &lt;/td&gt;</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L20" t="str" cm="1">
+        <f t="array" ref="L20">INDEX(K$6:K$107,ROWS(K20:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2014 &lt;/td&gt;</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
+      </c>
+      <c r="L21" t="str" cm="1">
+        <f t="array" ref="L21">INDEX(K$6:K$107,ROWS(K21:K$107))</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q8, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 12-0 &lt;/td&gt;</v>
+      </c>
+      <c r="L22" t="str" cm="1">
+        <f t="array" ref="L22">INDEX(K$6:K$107,ROWS(K22:K$107))</f>
+        <v>&lt;td&gt;Final 14-7 &lt;/td&gt;</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L23" t="str" cm="1">
+        <f t="array" ref="L23">INDEX(K$6:K$107,ROWS(K23:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 2013 &lt;/td&gt;</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="K24" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
+      </c>
+      <c r="L24" t="str" cm="1">
+        <f t="array" ref="L24">INDEX(K$6:K$107,ROWS(K24:K$107))</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O11, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 18-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L25" t="str" cm="1">
+        <f t="array" ref="L25">INDEX(K$6:K$107,ROWS(K25:K$107))</f>
+        <v>&lt;td&gt;Final 38-10 &lt;/td&gt;</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L26" t="str" cm="1">
+        <f t="array" ref="L26">INDEX(K$6:K$107,ROWS(K26:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Rotorua 2012 &lt;/td&gt;</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="P26" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q26" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
+      </c>
+      <c r="L27" t="str" cm="1">
+        <f t="array" ref="L27">INDEX(K$6:K$107,ROWS(K27:K$107))</f>
+        <v>&lt;td&gt;1. Tauranga Boys’ College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P11, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 9-6 &lt;/td&gt;</v>
+      </c>
+      <c r="L28" t="str" cm="1">
+        <f t="array" ref="L28">INDEX(K$6:K$107,ROWS(K28:K$107))</f>
+        <v>&lt;td&gt;Final 10-7 &lt;/td&gt;</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L29" t="str" cm="1">
+        <f t="array" ref="L29">INDEX(K$6:K$107,ROWS(K29:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hastings 2011 &lt;/td&gt;</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
+      </c>
+      <c r="L30" t="str" cm="1">
+        <f t="array" ref="L30">INDEX(K$6:K$107,ROWS(K30:K$107))</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q11, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 20-0 &lt;/td&gt;</v>
+      </c>
+      <c r="L31" t="str" cm="1">
+        <f t="array" ref="L31">INDEX(K$6:K$107,ROWS(K31:K$107))</f>
+        <v>&lt;td&gt;Final 14-6 &lt;/td&gt;</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K32" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L32" t="str" cm="1">
+        <f t="array" ref="L32">INDEX(K$6:K$107,ROWS(K32:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;St Bede’s 2010 &lt;/td&gt;</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
+      </c>
+      <c r="L33" t="str" cm="1">
+        <f t="array" ref="L33">INDEX(K$6:K$107,ROWS(K33:K$107))</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q33" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O14, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 26-0 &lt;/td&gt;</v>
+      </c>
+      <c r="L34" t="str" cm="1">
+        <f t="array" ref="L34">INDEX(K$6:K$107,ROWS(K34:K$107))</f>
+        <v>&lt;td&gt;Final 24-5 &lt;/td&gt;</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="P34" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q34" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="K35" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O15, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L35" t="str" cm="1">
+        <f t="array" ref="L35">INDEX(K$6:K$107,ROWS(K35:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;New Plymouth 2009 &lt;/td&gt;</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
+      </c>
+      <c r="L36" t="str" cm="1">
+        <f t="array" ref="L36">INDEX(K$6:K$107,ROWS(K36:K$107))</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q36" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="K37" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P14, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 9-5 &lt;/td&gt;</v>
+      </c>
+      <c r="L37" t="str" cm="1">
+        <f t="array" ref="L37">INDEX(K$6:K$107,ROWS(K37:K$107))</f>
+        <v>&lt;td&gt;Final 20-3 &lt;/td&gt;</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+    </row>
+    <row r="38" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P15, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L38" t="str" cm="1">
+        <f t="array" ref="L38">INDEX(K$6:K$107,ROWS(K38:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2008 &lt;/td&gt;</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+    </row>
+    <row r="39" spans="2:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="K39" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
+      </c>
+      <c r="L39" t="str" cm="1">
+        <f t="array" ref="L39">INDEX(K$6:K$107,ROWS(K39:K$107))</f>
+        <v>&lt;td&gt;1. Palmerston North BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+    </row>
+    <row r="40" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K40" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q14, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 22-5 &lt;/td&gt;</v>
+      </c>
+      <c r="L40" t="str" cm="1">
+        <f t="array" ref="L40">INDEX(K$6:K$107,ROWS(K40:K$107))</f>
+        <v>&lt;td&gt;Final 18-15 &lt;/td&gt;</v>
+      </c>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+    </row>
+    <row r="41" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="K41" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q15, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L41" t="str" cm="1">
+        <f t="array" ref="L41">INDEX(K$6:K$107,ROWS(K41:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
+      </c>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K42" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
+      </c>
+      <c r="L42" t="str" cm="1">
+        <f t="array" ref="L42">INDEX(K$6:K$107,ROWS(K42:K$107))</f>
+        <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+      <c r="K43" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O17, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 16-13 &lt;/td&gt;</v>
+      </c>
+      <c r="L43" t="str" cm="1">
+        <f t="array" ref="L43">INDEX(K$6:K$107,ROWS(K43:K$107))</f>
+        <v>&lt;td&gt;Final 15-0 &lt;/td&gt;</v>
+      </c>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K44" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L44" t="str" cm="1">
+        <f t="array" ref="L44">INDEX(K$6:K$107,ROWS(K44:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
+      </c>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+    </row>
+    <row r="45" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
+      </c>
+      <c r="L45" t="str" cm="1">
+        <f t="array" ref="L45">INDEX(K$6:K$107,ROWS(K45:K$107))</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+    </row>
+    <row r="46" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P17, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 14-13 &lt;/td&gt;</v>
+      </c>
+      <c r="L46" t="str" cm="1">
+        <f t="array" ref="L46">INDEX(K$6:K$107,ROWS(K46:K$107))</f>
+        <v>&lt;td&gt;Final 20-12 &lt;/td&gt;</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+    </row>
+    <row r="47" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="K47" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L47" t="str" cm="1">
+        <f t="array" ref="L47">INDEX(K$6:K$107,ROWS(K47:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 2005 &lt;/td&gt;</v>
+      </c>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+    </row>
+    <row r="48" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
+      </c>
+      <c r="L48" t="str" cm="1">
+        <f t="array" ref="L48">INDEX(K$6:K$107,ROWS(K48:K$107))</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+    </row>
+    <row r="49" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
+      <c r="K49" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q17, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 13-12 &lt;/td&gt;</v>
+      </c>
+      <c r="L49" t="str" cm="1">
+        <f t="array" ref="L49">INDEX(K$6:K$107,ROWS(K49:K$107))</f>
+        <v>&lt;td&gt;Final 47-0 &lt;/td&gt;</v>
+      </c>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+    </row>
+    <row r="50" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K50" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L50" t="str" cm="1">
+        <f t="array" ref="L50">INDEX(K$6:K$107,ROWS(K50:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 2004 &lt;/td&gt;</v>
+      </c>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+    </row>
+    <row r="51" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+      <c r="K51" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
+      </c>
+      <c r="L51" t="str" cm="1">
+        <f t="array" ref="L51">INDEX(K$6:K$107,ROWS(K51:K$107))</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+    </row>
+    <row r="52" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K52" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O20, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 18-7 &lt;/td&gt;</v>
+      </c>
+      <c r="L52" t="str" cm="1">
+        <f t="array" ref="L52">INDEX(K$6:K$107,ROWS(K52:K$107))</f>
+        <v>&lt;td&gt;Final 22-14 &lt;/td&gt;</v>
+      </c>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+    </row>
+    <row r="53" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="K53" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L53" t="str" cm="1">
+        <f t="array" ref="L53">INDEX(K$6:K$107,ROWS(K53:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 2003 &lt;/td&gt;</v>
+      </c>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+    </row>
+    <row r="54" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
+      </c>
+      <c r="L54" t="str" cm="1">
+        <f t="array" ref="L54">INDEX(K$6:K$107,ROWS(K54:K$107))</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+    </row>
+    <row r="55" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+      <c r="K55" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P20, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 27-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L55" t="str" cm="1">
+        <f t="array" ref="L55">INDEX(K$6:K$107,ROWS(K55:K$107))</f>
+        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+    </row>
+    <row r="56" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L56" t="str" cm="1">
+        <f t="array" ref="L56">INDEX(K$6:K$107,ROWS(K56:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
+      </c>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+    </row>
+    <row r="57" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="K57" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
+      </c>
+      <c r="L57" t="str" cm="1">
+        <f t="array" ref="L57">INDEX(K$6:K$107,ROWS(K57:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+    </row>
+    <row r="58" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K58" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q20, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L58" t="str" cm="1">
+        <f t="array" ref="L58">INDEX(K$6:K$107,ROWS(K58:K$107))</f>
+        <v>&lt;td&gt;Final 27-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+    </row>
+    <row r="59" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
+      <c r="K59" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L59" t="str" cm="1">
+        <f t="array" ref="L59">INDEX(K$6:K$107,ROWS(K59:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
+      </c>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+    </row>
+    <row r="60" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K60" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 2003 &lt;/td&gt;</v>
+      </c>
+      <c r="L60" t="str" cm="1">
+        <f t="array" ref="L60">INDEX(K$6:K$107,ROWS(K60:K$107))</f>
+        <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
+      <c r="K61" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O23, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 22-14 &lt;/td&gt;</v>
+      </c>
+      <c r="L61" t="str" cm="1">
+        <f t="array" ref="L61">INDEX(K$6:K$107,ROWS(K61:K$107))</f>
+        <v>&lt;td&gt;Final 18-7 &lt;/td&gt;</v>
+      </c>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K62" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L62" t="str" cm="1">
+        <f t="array" ref="L62">INDEX(K$6:K$107,ROWS(K62:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
+      </c>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
+      <c r="K63" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 2004 &lt;/td&gt;</v>
+      </c>
+      <c r="L63" t="str" cm="1">
+        <f t="array" ref="L63">INDEX(K$6:K$107,ROWS(K63:K$107))</f>
+        <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+    </row>
+    <row r="64" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K64" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P23, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 47-0 &lt;/td&gt;</v>
+      </c>
+      <c r="L64" t="str" cm="1">
+        <f t="array" ref="L64">INDEX(K$6:K$107,ROWS(K64:K$107))</f>
+        <v>&lt;td&gt;Final 13-12 &lt;/td&gt;</v>
+      </c>
+      <c r="M64" s="10"/>
+      <c r="N64" s="10"/>
+    </row>
+    <row r="65" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K65" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L65" t="str" cm="1">
+        <f t="array" ref="L65">INDEX(K$6:K$107,ROWS(K65:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
+      </c>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+    </row>
+    <row r="66" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 2005 &lt;/td&gt;</v>
+      </c>
+      <c r="L66" t="str" cm="1">
+        <f t="array" ref="L66">INDEX(K$6:K$107,ROWS(K66:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+    </row>
+    <row r="67" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
+      <c r="K67" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q23, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 20-12 &lt;/td&gt;</v>
+      </c>
+      <c r="L67" t="str" cm="1">
+        <f t="array" ref="L67">INDEX(K$6:K$107,ROWS(K67:K$107))</f>
+        <v>&lt;td&gt;Final 14-13 &lt;/td&gt;</v>
+      </c>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+    </row>
+    <row r="68" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L68" t="str" cm="1">
+        <f t="array" ref="L68">INDEX(K$6:K$107,ROWS(K68:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
+      </c>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+    </row>
+    <row r="69" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
+      <c r="K69" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
+      </c>
+      <c r="L69" t="str" cm="1">
+        <f t="array" ref="L69">INDEX(K$6:K$107,ROWS(K69:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+    </row>
+    <row r="70" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K70" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O26, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 15-0 &lt;/td&gt;</v>
+      </c>
+      <c r="L70" t="str" cm="1">
+        <f t="array" ref="L70">INDEX(K$6:K$107,ROWS(K70:K$107))</f>
+        <v>&lt;td&gt;Final 16-13 &lt;/td&gt;</v>
+      </c>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+    </row>
+    <row r="71" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
+      <c r="K71" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L71" t="str" cm="1">
+        <f t="array" ref="L71">INDEX(K$6:K$107,ROWS(K71:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
+      </c>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+    </row>
+    <row r="72" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K72" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
+      </c>
+      <c r="L72" t="str" cm="1">
+        <f t="array" ref="L72">INDEX(K$6:K$107,ROWS(K72:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+    </row>
+    <row r="73" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
+      <c r="K73" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P26, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 18-15 &lt;/td&gt;</v>
+      </c>
+      <c r="L73" t="str" cm="1">
+        <f t="array" ref="L73">INDEX(K$6:K$107,ROWS(K73:K$107))</f>
+        <v>&lt;td&gt;Final 22-5 &lt;/td&gt;</v>
+      </c>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+    </row>
+    <row r="74" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K74" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Palmerston North BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L74" t="str" cm="1">
+        <f t="array" ref="L74">INDEX(K$6:K$107,ROWS(K74:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
+      </c>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+    </row>
+    <row r="75" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
+      <c r="K75" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2008 &lt;/td&gt;</v>
+      </c>
+      <c r="L75" t="str" cm="1">
+        <f t="array" ref="L75">INDEX(K$6:K$107,ROWS(K75:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+    </row>
+    <row r="76" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K76" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q26, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 20-3 &lt;/td&gt;</v>
+      </c>
+      <c r="L76" t="str" cm="1">
+        <f t="array" ref="L76">INDEX(K$6:K$107,ROWS(K76:K$107))</f>
+        <v>&lt;td&gt;Final 9-5 &lt;/td&gt;</v>
+      </c>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+    </row>
+    <row r="77" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
+      <c r="K77" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L77" t="str" cm="1">
+        <f t="array" ref="L77">INDEX(K$6:K$107,ROWS(K77:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
+      </c>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+    </row>
+    <row r="78" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K78" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;New Plymouth 2009 &lt;/td&gt;</v>
+      </c>
+      <c r="L78" t="str" cm="1">
+        <f t="array" ref="L78">INDEX(K$6:K$107,ROWS(K78:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+    </row>
+    <row r="79" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
+      <c r="K79" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O29, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 24-5 &lt;/td&gt;</v>
+      </c>
+      <c r="L79" t="str" cm="1">
+        <f t="array" ref="L79">INDEX(K$6:K$107,ROWS(K79:K$107))</f>
+        <v>&lt;td&gt;Final 26-0 &lt;/td&gt;</v>
+      </c>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K80" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L80" t="str" cm="1">
+        <f t="array" ref="L80">INDEX(K$6:K$107,ROWS(K80:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
+      </c>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="K81" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;St Bede’s 2010 &lt;/td&gt;</v>
+      </c>
+      <c r="L81" t="str" cm="1">
+        <f t="array" ref="L81">INDEX(K$6:K$107,ROWS(K81:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M81" s="11"/>
+      <c r="N81" s="11"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K82" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P29, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 14-6 &lt;/td&gt;</v>
+      </c>
+      <c r="L82" t="str" cm="1">
+        <f t="array" ref="L82">INDEX(K$6:K$107,ROWS(K82:K$107))</f>
+        <v>&lt;td&gt;Final 20-0 &lt;/td&gt;</v>
+      </c>
+      <c r="M82" s="11"/>
+      <c r="N82" s="11"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K83" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L83" t="str" cm="1">
+        <f t="array" ref="L83">INDEX(K$6:K$107,ROWS(K83:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
+      </c>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+    </row>
+    <row r="84" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K84" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hastings 2011 &lt;/td&gt;</v>
+      </c>
+      <c r="L84" t="str" cm="1">
+        <f t="array" ref="L84">INDEX(K$6:K$107,ROWS(K84:K$107))</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+    </row>
+    <row r="85" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K85" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q29, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 10-7 &lt;/td&gt;</v>
+      </c>
+      <c r="L85" t="str" cm="1">
+        <f t="array" ref="L85">INDEX(K$6:K$107,ROWS(K85:K$107))</f>
+        <v>&lt;td&gt;Final 9-6 &lt;/td&gt;</v>
+      </c>
+      <c r="M85" s="10"/>
+      <c r="N85" s="10"/>
+    </row>
+    <row r="86" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K86" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Tauranga Boys’ College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L86" t="str" cm="1">
+        <f t="array" ref="L86">INDEX(K$6:K$107,ROWS(K86:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
+      </c>
+      <c r="M86" s="10"/>
+      <c r="N86" s="10"/>
+    </row>
+    <row r="87" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K87" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Rotorua 2012 &lt;/td&gt;</v>
+      </c>
+      <c r="L87" t="str" cm="1">
+        <f t="array" ref="L87">INDEX(K$6:K$107,ROWS(K87:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M87" s="10"/>
+      <c r="N87" s="10"/>
+    </row>
+    <row r="88" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K88" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O32, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 38-10 &lt;/td&gt;</v>
+      </c>
+      <c r="L88" t="str" cm="1">
+        <f t="array" ref="L88">INDEX(K$6:K$107,ROWS(K88:K$107))</f>
+        <v>&lt;td&gt;Final 18-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+    </row>
+    <row r="89" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K89" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L89" t="str" cm="1">
+        <f t="array" ref="L89">INDEX(K$6:K$107,ROWS(K89:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
+      </c>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+    </row>
+    <row r="90" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K90" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 2013 &lt;/td&gt;</v>
+      </c>
+      <c r="L90" t="str" cm="1">
+        <f t="array" ref="L90">INDEX(K$6:K$107,ROWS(K90:K$107))</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+    </row>
+    <row r="91" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K91" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P32, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 14-7 &lt;/td&gt;</v>
+      </c>
+      <c r="L91" t="str" cm="1">
+        <f t="array" ref="L91">INDEX(K$6:K$107,ROWS(K91:K$107))</f>
+        <v>&lt;td&gt;Final 12-0 &lt;/td&gt;</v>
+      </c>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+    </row>
+    <row r="92" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K92" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L92" t="str" cm="1">
+        <f t="array" ref="L92">INDEX(K$6:K$107,ROWS(K92:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
+      </c>
+      <c r="M92" s="10"/>
+      <c r="N92" s="10"/>
+    </row>
+    <row r="93" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K93" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2014 &lt;/td&gt;</v>
+      </c>
+      <c r="L93" t="str" cm="1">
+        <f t="array" ref="L93">INDEX(K$6:K$107,ROWS(K93:K$107))</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+    </row>
+    <row r="94" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K94" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q32, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 27-26 &lt;/td&gt;</v>
+      </c>
+      <c r="L94" t="str" cm="1">
+        <f t="array" ref="L94">INDEX(K$6:K$107,ROWS(K94:K$107))</f>
+        <v>&lt;td&gt;Final 6-4 &lt;/td&gt;</v>
+      </c>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+    </row>
+    <row r="95" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K95" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L95" t="str" cm="1">
+        <f t="array" ref="L95">INDEX(K$6:K$107,ROWS(K95:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
+      </c>
+      <c r="M95" s="10"/>
+      <c r="N95" s="10"/>
+    </row>
+    <row r="96" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K96" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2015 &lt;/td&gt;</v>
+      </c>
+      <c r="L96" t="str" cm="1">
+        <f t="array" ref="L96">INDEX(K$6:K$107,ROWS(K96:K$107))</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M96" s="10"/>
+      <c r="N96" s="10"/>
+    </row>
+    <row r="97" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K97" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O35, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final &lt;/td&gt;</v>
+      </c>
+      <c r="L97" t="str" cm="1">
+        <f t="array" ref="L97">INDEX(K$6:K$107,ROWS(K97:K$107))</f>
+        <v>&lt;td&gt;Final 17-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M97" s="10"/>
+      <c r="N97" s="10"/>
+    </row>
+    <row r="98" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K98" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1.Wesley College &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L98" t="str" cm="1">
+        <f t="array" ref="L98">INDEX(K$6:K$107,ROWS(K98:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>
+      </c>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+    </row>
+    <row r="99" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K99" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Massey High School 2016 &lt;/td&gt;</v>
+      </c>
+      <c r="L99" t="str" cm="1">
+        <f t="array" ref="L99">INDEX(K$6:K$107,ROWS(K99:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M99" s="10"/>
+      <c r="N99" s="10"/>
+    </row>
+    <row r="100" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K100" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P35, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final &lt;/td&gt;</v>
+      </c>
+      <c r="L100" t="str" cm="1">
+        <f t="array" ref="L100">INDEX(K$6:K$107,ROWS(K100:K$107))</f>
+        <v>&lt;td&gt;Final 12-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M100" s="11"/>
+      <c r="N100" s="11"/>
+    </row>
+    <row r="101" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K101" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1.Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L101" t="str" cm="1">
+        <f t="array" ref="L101">INDEX(K$6:K$107,ROWS(K101:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
+      </c>
+      <c r="M101" s="11"/>
+      <c r="N101" s="11"/>
+    </row>
+    <row r="102" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K102" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2017 &lt;/td&gt;</v>
+      </c>
+      <c r="L102" t="str" cm="1">
+        <f t="array" ref="L102">INDEX(K$6:K$107,ROWS(K102:K$107))</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M102" s="11"/>
+      <c r="N102" s="11"/>
+    </row>
+    <row r="103" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K103" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q35, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 22-18 &lt;/td&gt;</v>
+      </c>
+      <c r="L103" t="str" cm="1">
+        <f t="array" ref="L103">INDEX(K$6:K$107,ROWS(K103:K$107))</f>
+        <v>&lt;td&gt;Final 8-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M103" s="10"/>
+      <c r="N103" s="10"/>
+    </row>
+    <row r="104" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K104" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L104" t="str" cm="1">
+        <f t="array" ref="L104">INDEX(K$6:K$107,ROWS(K104:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1986 &lt;/td&gt;</v>
+      </c>
+      <c r="M104" s="10"/>
+      <c r="N104" s="10"/>
+    </row>
+    <row r="105" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K105" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O37, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland Grammar 2018&lt;/td&gt;</v>
+      </c>
+      <c r="L105" t="str" cm="1">
+        <f t="array" ref="L105">INDEX(K$6:K$107,ROWS(K105:K$107))</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M105" s="10"/>
+      <c r="N105" s="10"/>
+    </row>
+    <row r="106" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K106" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O38, "&lt;/td&gt;")</f>
+        <v>&lt;td&gt;Final 17-21&lt;/td&gt;</v>
+      </c>
+      <c r="L106" t="str" cm="1">
+        <f t="array" ref="L106">INDEX(K$6:K$107,ROWS(K106:K$107))</f>
+        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+      </c>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10"/>
+    </row>
+    <row r="107" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K107" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O39, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="L107" t="str" cm="1">
+        <f t="array" ref="L107">INDEX(K$6:K$107,ROWS(K107:K$107))</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1985 &lt;/td&gt;</v>
+      </c>
+      <c r="M107" s="10"/>
+      <c r="N107" s="10"/>
+    </row>
+    <row r="108" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L108" s="10"/>
+      <c r="M108" s="10"/>
+      <c r="N108" s="10"/>
+    </row>
+    <row r="109" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L109" s="10"/>
+      <c r="M109" s="10"/>
+      <c r="N109" s="10"/>
+    </row>
+    <row r="110" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L110" s="10"/>
+      <c r="M110" s="10"/>
+      <c r="N110" s="10"/>
+    </row>
+    <row r="111" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L111" s="10"/>
+      <c r="M111" s="10"/>
+      <c r="N111" s="10"/>
+    </row>
+    <row r="112" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L112" s="10"/>
+      <c r="M112" s="10"/>
+      <c r="N112" s="10"/>
+    </row>
+    <row r="113" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L113" s="10"/>
+      <c r="M113" s="10"/>
+      <c r="N113" s="10"/>
+    </row>
+    <row r="114" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L114" s="10"/>
+      <c r="M114" s="10"/>
+      <c r="N114" s="10"/>
+    </row>
+    <row r="115" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L115" s="10"/>
+      <c r="M115" s="10"/>
+      <c r="N115" s="10"/>
+    </row>
+    <row r="116" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L116" s="10"/>
+      <c r="M116" s="10"/>
+      <c r="N116" s="10"/>
+    </row>
+    <row r="117" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L117" s="10"/>
+      <c r="M117" s="10"/>
+      <c r="N117" s="10"/>
+    </row>
+    <row r="118" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L118" s="12"/>
+      <c r="M118" s="12"/>
+      <c r="N118" s="10"/>
+    </row>
+    <row r="119" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L119" s="11"/>
+      <c r="M119" s="14"/>
+      <c r="N119" s="14"/>
+    </row>
+    <row r="120" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L120" s="11"/>
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+    </row>
+    <row r="121" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L121" s="11"/>
+      <c r="M121" s="14"/>
+      <c r="N121" s="14"/>
+    </row>
+    <row r="122" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L122" s="10"/>
+      <c r="M122" s="14"/>
+      <c r="N122" s="14"/>
+    </row>
+    <row r="123" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L123" s="10"/>
+      <c r="M123" s="14"/>
+      <c r="N123" s="14"/>
+    </row>
+    <row r="124" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L124" s="10"/>
+      <c r="M124" s="14"/>
+      <c r="N124" s="14"/>
+    </row>
+    <row r="125" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L125" s="10"/>
+      <c r="M125" s="14"/>
+      <c r="N125" s="14"/>
+    </row>
+    <row r="126" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L126" s="10"/>
+      <c r="M126" s="14"/>
+      <c r="N126" s="14"/>
+    </row>
+    <row r="127" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L127" s="10"/>
+      <c r="M127" s="14"/>
+      <c r="N127" s="14"/>
+    </row>
+    <row r="128" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L128" s="10"/>
+      <c r="M128" s="14"/>
+      <c r="N128" s="14"/>
+    </row>
+    <row r="129" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L129" s="10"/>
+      <c r="M129" s="14"/>
+      <c r="N129" s="14"/>
+    </row>
+    <row r="130" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L130" s="10"/>
+      <c r="M130" s="14"/>
+      <c r="N130" s="14"/>
+    </row>
+    <row r="131" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L131" s="10"/>
+      <c r="M131" s="14"/>
+      <c r="N131" s="14"/>
+    </row>
+    <row r="132" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L132" s="10"/>
+      <c r="M132" s="14"/>
+      <c r="N132" s="14"/>
+    </row>
+    <row r="133" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L133" s="10"/>
+      <c r="M133" s="14"/>
+      <c r="N133" s="14"/>
+    </row>
+    <row r="134" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L134" s="10"/>
+      <c r="M134" s="14"/>
+      <c r="N134" s="14"/>
+    </row>
+    <row r="135" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L135" s="10"/>
+      <c r="M135" s="14"/>
+      <c r="N135" s="14"/>
+    </row>
+    <row r="136" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L136" s="10"/>
+      <c r="M136" s="14"/>
+      <c r="N136" s="14"/>
+    </row>
+    <row r="137" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L137" s="11"/>
+      <c r="M137" s="11"/>
+      <c r="N137" s="11"/>
+    </row>
+    <row r="138" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L138" s="11"/>
+      <c r="M138" s="11"/>
+      <c r="N138" s="11"/>
+    </row>
+    <row r="139" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L139" s="11"/>
+      <c r="M139" s="11"/>
+      <c r="N139" s="11"/>
+    </row>
+    <row r="140" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L140" s="11"/>
+      <c r="M140" s="11"/>
+      <c r="N140" s="11"/>
+    </row>
+    <row r="141" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L141" s="11"/>
+      <c r="M141" s="11"/>
+      <c r="N141" s="11"/>
+    </row>
+    <row r="142" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L142" s="11"/>
+      <c r="M142" s="11"/>
+      <c r="N142" s="11"/>
+    </row>
+    <row r="143" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L143" s="11"/>
+      <c r="M143" s="11"/>
+      <c r="N143" s="11"/>
+    </row>
+    <row r="144" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L144" s="11"/>
+      <c r="M144" s="11"/>
+      <c r="N144" s="11"/>
+    </row>
+    <row r="145" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L145" s="11"/>
+      <c r="M145" s="11"/>
+      <c r="N145" s="11"/>
+    </row>
+    <row r="146" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L146" s="11"/>
+      <c r="M146" s="11"/>
+      <c r="N146" s="11"/>
+    </row>
+    <row r="147" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L147" s="11"/>
+      <c r="M147" s="11"/>
+      <c r="N147" s="11"/>
+    </row>
+    <row r="148" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L148" s="11"/>
+      <c r="M148" s="11"/>
+      <c r="N148" s="11"/>
+    </row>
+    <row r="149" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L149" s="11"/>
+      <c r="M149" s="11"/>
+      <c r="N149" s="11"/>
+    </row>
+    <row r="150" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L150" s="11"/>
+      <c r="M150" s="11"/>
+      <c r="N150" s="11"/>
+    </row>
+    <row r="151" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L151" s="11"/>
+      <c r="M151" s="11"/>
+      <c r="N151" s="11"/>
+    </row>
+    <row r="152" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L152" s="11"/>
+      <c r="M152" s="11"/>
+      <c r="N152" s="11"/>
+    </row>
+    <row r="153" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L153" s="11"/>
+      <c r="M153" s="11"/>
+      <c r="N153" s="11"/>
+    </row>
+    <row r="154" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L154" s="11"/>
+      <c r="M154" s="11"/>
+      <c r="N154" s="11"/>
+    </row>
+    <row r="155" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L155" s="11"/>
+      <c r="M155" s="11"/>
+      <c r="N155" s="11"/>
+    </row>
+    <row r="156" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L156" s="11"/>
+      <c r="M156" s="11"/>
+      <c r="N156" s="11"/>
+    </row>
+    <row r="157" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L157" s="11"/>
+      <c r="M157" s="11"/>
+      <c r="N157" s="11"/>
+    </row>
+    <row r="158" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L158" s="11"/>
+      <c r="M158" s="11"/>
+      <c r="N158" s="11"/>
+    </row>
+    <row r="159" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L159" s="11"/>
+      <c r="M159" s="11"/>
+      <c r="N159" s="11"/>
+    </row>
+    <row r="160" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L160" s="11"/>
+      <c r="M160" s="11"/>
+      <c r="N160" s="11"/>
+    </row>
+    <row r="161" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L161" s="11"/>
+      <c r="M161" s="11"/>
+      <c r="N161" s="11"/>
+    </row>
+    <row r="162" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L162" s="11"/>
+      <c r="M162" s="11"/>
+      <c r="N162" s="11"/>
+    </row>
+    <row r="163" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L163" s="11"/>
+      <c r="M163" s="11"/>
+      <c r="N163" s="11"/>
+    </row>
+    <row r="164" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L164" s="11"/>
+      <c r="M164" s="11"/>
+      <c r="N164" s="11"/>
+    </row>
+    <row r="165" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L165" s="11"/>
+      <c r="M165" s="11"/>
+      <c r="N165" s="11"/>
+    </row>
+    <row r="166" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L166" s="11"/>
+      <c r="M166" s="11"/>
+      <c r="N166" s="11"/>
+    </row>
+    <row r="167" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L167" s="11"/>
+      <c r="M167" s="11"/>
+      <c r="N167" s="11"/>
+    </row>
+    <row r="168" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L168" s="11"/>
+      <c r="M168" s="11"/>
+      <c r="N168" s="11"/>
+    </row>
+    <row r="169" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L169" s="11"/>
+      <c r="M169" s="11"/>
+      <c r="N169" s="11"/>
+    </row>
+    <row r="170" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L170" s="11"/>
+      <c r="M170" s="11"/>
+      <c r="N170" s="11"/>
+    </row>
+    <row r="171" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L171" s="11"/>
+      <c r="M171" s="11"/>
+      <c r="N171" s="11"/>
+    </row>
+    <row r="172" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L172" s="11"/>
+      <c r="M172" s="11"/>
+      <c r="N172" s="11"/>
+    </row>
+    <row r="173" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L173" s="11"/>
+      <c r="M173" s="11"/>
+      <c r="N173" s="11"/>
+    </row>
+    <row r="174" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L174" s="11"/>
+      <c r="M174" s="11"/>
+      <c r="N174" s="11"/>
+    </row>
+    <row r="175" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L175" s="11"/>
+      <c r="M175" s="11"/>
+      <c r="N175" s="11"/>
+    </row>
+    <row r="176" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L176" s="11"/>
+      <c r="M176" s="11"/>
+      <c r="N176" s="11"/>
+    </row>
+    <row r="177" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L177" s="11"/>
+      <c r="M177" s="11"/>
+      <c r="N177" s="11"/>
+    </row>
+    <row r="178" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L178" s="11"/>
+      <c r="M178" s="11"/>
+      <c r="N178" s="11"/>
+    </row>
+    <row r="179" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L179" s="11"/>
+      <c r="M179" s="11"/>
+      <c r="N179" s="11"/>
+    </row>
+    <row r="180" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L180" s="11"/>
+      <c r="M180" s="11"/>
+      <c r="N180" s="11"/>
+    </row>
+    <row r="181" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L181" s="11"/>
+      <c r="M181" s="11"/>
+      <c r="N181" s="11"/>
+    </row>
+    <row r="182" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L182" s="11"/>
+      <c r="M182" s="11"/>
+      <c r="N182" s="11"/>
+    </row>
+    <row r="183" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L183" s="11"/>
+      <c r="M183" s="11"/>
+      <c r="N183" s="11"/>
+    </row>
+    <row r="184" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L184" s="11"/>
+      <c r="M184" s="11"/>
+      <c r="N184" s="11"/>
+    </row>
+    <row r="185" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L185" s="11"/>
+      <c r="M185" s="11"/>
+      <c r="N185" s="11"/>
+    </row>
+    <row r="186" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L186" s="11"/>
+      <c r="M186" s="11"/>
+      <c r="N186" s="11"/>
+    </row>
+    <row r="187" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L187" s="11"/>
+      <c r="M187" s="11"/>
+      <c r="N187" s="11"/>
+    </row>
+    <row r="188" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L188" s="11"/>
+      <c r="M188" s="11"/>
+      <c r="N188" s="11"/>
+    </row>
+    <row r="189" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L189" s="11"/>
+      <c r="M189" s="11"/>
+      <c r="N189" s="11"/>
+    </row>
+    <row r="190" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L190" s="11"/>
+      <c r="M190" s="11"/>
+      <c r="N190" s="11"/>
+    </row>
+    <row r="191" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L191" s="11"/>
+      <c r="M191" s="11"/>
+      <c r="N191" s="11"/>
+    </row>
+    <row r="192" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L192" s="11"/>
+      <c r="M192" s="11"/>
+      <c r="N192" s="11"/>
+    </row>
+    <row r="193" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L193" s="11"/>
+      <c r="M193" s="11"/>
+      <c r="N193" s="11"/>
+    </row>
+    <row r="194" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L194" s="11"/>
+      <c r="M194" s="11"/>
+      <c r="N194" s="11"/>
+    </row>
+    <row r="195" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L195" s="11"/>
+      <c r="M195" s="11"/>
+      <c r="N195" s="11"/>
+    </row>
+    <row r="196" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L196" s="11"/>
+      <c r="M196" s="11"/>
+      <c r="N196" s="11"/>
+    </row>
+    <row r="197" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L197" s="11"/>
+      <c r="M197" s="11"/>
+      <c r="N197" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M119:M136"/>
+    <mergeCell ref="N119:N136"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
made the tabs work this fixes #41
Signed-off-by: YelloElefant <alextrotternz@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F19FDBB1-E2BD-4B39-96FE-3D4605BB12B4}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6ACE38-6804-48F7-A265-138722ED4978}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-18000" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
+    <workbookView xWindow="-28920" yWindow="-2670" windowWidth="29040" windowHeight="15840" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="181">
   <si>
     <r>
       <t>&lt;</t>
@@ -3059,13 +3059,103 @@
   </si>
   <si>
     <t>1. Hamilton BHS</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Auckland Grammar School</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Mt. Albert Grammar School</t>
+  </si>
+  <si>
+    <t>2.30pm</t>
+  </si>
+  <si>
+    <t>MARIST 2</t>
+  </si>
+  <si>
+    <t>Palmerston North BHS</t>
+  </si>
+  <si>
+    <t>St. Bedes College</t>
+  </si>
+  <si>
+    <t>MARIST 1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Westlake BHS</t>
+  </si>
+  <si>
+    <t>New Plymouth BHS</t>
+  </si>
+  <si>
+    <t>MARIST 3</t>
+  </si>
+  <si>
+    <t>Rotorua BHS</t>
+  </si>
+  <si>
+    <t>St Pats Town</t>
+  </si>
+  <si>
+    <t>HBHS 3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Hastings BHS</t>
+  </si>
+  <si>
+    <t>Otago BHS</t>
+  </si>
+  <si>
+    <t>HBHS 2</t>
+  </si>
+  <si>
+    <t>Hamilton BHS</t>
+  </si>
+  <si>
+    <t>Napier BHS</t>
+  </si>
+  <si>
+    <t>HBHS 1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Christchurch BHS</t>
+  </si>
+  <si>
+    <t>Wellington College</t>
+  </si>
+  <si>
+    <t>UNI 1</t>
+  </si>
+  <si>
+    <t>Tauranga Boys College</t>
+  </si>
+  <si>
+    <t>Wesley College</t>
+  </si>
+  <si>
+    <t>UNI 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3112,16 +3202,43 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -3173,11 +3290,190 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3204,19 +3500,77 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3232,6 +3586,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3531,10 +3889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD87F2E1-A52F-4456-AB4D-EECF95DE5FBF}">
-  <dimension ref="B3:Q197"/>
+  <dimension ref="B3:Y136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L107" sqref="L6:L107"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13:Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,10 +3907,17 @@
     <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="H4" s="3" t="s">
         <v>65</v>
       </c>
@@ -3565,8 +3930,29 @@
       <c r="Q4" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S4" s="14">
+        <v>9</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3585,8 +3971,29 @@
       <c r="Q5" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S5" s="14">
+        <v>10</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="V5" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y5" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3613,8 +4020,29 @@
       <c r="Q6" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S6" s="14">
+        <v>11</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="U6" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="W6" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="X6" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y6" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -3638,8 +4066,29 @@
       <c r="Q7" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S7" s="14">
+        <v>12</v>
+      </c>
+      <c r="T7" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="U7" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="W7" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="X7" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y7" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3663,8 +4112,29 @@
       <c r="Q8" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="S8" s="27">
+        <v>13</v>
+      </c>
+      <c r="T8" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="U8" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="V8" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="W8" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="X8" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y8" s="31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
@@ -3685,8 +4155,29 @@
       <c r="Q9" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S9" s="27">
+        <v>14</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="U9" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="W9" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="X9" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y9" s="35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -3710,8 +4201,29 @@
       <c r="Q10" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S10" s="14">
+        <v>15</v>
+      </c>
+      <c r="T10" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="U10" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="V10" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="W10" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="X10" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y10" s="35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
@@ -3735,8 +4247,29 @@
       <c r="Q11" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="27">
+        <v>16</v>
+      </c>
+      <c r="T11" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="U11" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="V11" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="W11" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="X11" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y11" s="35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -3761,7 +4294,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -3785,8 +4318,36 @@
       <c r="Q13" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S13" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;",S4,"&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;9&lt;/td&gt;</v>
+      </c>
+      <c r="T13" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T4,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;D&lt;/td&gt;</v>
+      </c>
+      <c r="U13" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("&lt;td class='teamLeft'&gt;",U4,"&lt;/td&gt;")</f>
+        <v>&lt;td class='teamLeft'&gt;Auckland Grammar School&lt;/td&gt;</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" ref="U13:Y13" si="0" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",V4,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W13" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("&lt;td class='teamRight'&gt;",W4,"&lt;/td&gt;")</f>
+        <v>&lt;td class='teamRight'&gt;Mt. Albert Grammar School&lt;/td&gt;</v>
+      </c>
+      <c r="X13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y13" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",Y4,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;MARIST 2&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>47</v>
       </c>
@@ -3807,8 +4368,36 @@
       <c r="Q14" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S14" t="str">
+        <f t="shared" ref="S14:S20" si="1" xml:space="preserve"> _xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;",S5,"&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;10&lt;/td&gt;</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" ref="T14:X14" si="2" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T5,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;D&lt;/td&gt;</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" ref="U14:U20" si="3" xml:space="preserve"> _xlfn.CONCAT("&lt;td class='teamLeft'&gt;",U5,"&lt;/td&gt;")</f>
+        <v>&lt;td class='teamLeft'&gt;Palmerston North BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" ref="W14:W20" si="4" xml:space="preserve"> _xlfn.CONCAT("&lt;td class='teamRight'&gt;",W5,"&lt;/td&gt;")</f>
+        <v>&lt;td class='teamRight'&gt;St. Bedes College&lt;/td&gt;</v>
+      </c>
+      <c r="X14" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" ref="Y14:Y20" si="5" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",Y5,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;MARIST 1&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
@@ -3832,8 +4421,36 @@
       <c r="Q15" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S15" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;11&lt;/td&gt;</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" ref="T15:X15" si="6" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T6,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;B&lt;/td&gt;</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Westlake BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;New Plymouth BHS&lt;/td&gt;</v>
+      </c>
+      <c r="X15" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;MARIST 3&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
@@ -3857,8 +4474,36 @@
       <c r="Q16" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S16" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;12&lt;/td&gt;</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" ref="T16:X16" si="7" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T7,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;B&lt;/td&gt;</v>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Rotorua BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;St Pats Town&lt;/td&gt;</v>
+      </c>
+      <c r="X16" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;HBHS 3&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -3882,8 +4527,36 @@
       <c r="Q17" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S17" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;13&lt;/td&gt;</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" ref="T17:X17" si="8" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T8,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;C&lt;/td&gt;</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Hastings BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;Otago BHS&lt;/td&gt;</v>
+      </c>
+      <c r="X17" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;HBHS 2&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -3907,8 +4580,36 @@
       <c r="Q18" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="S18" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;14&lt;/td&gt;</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" ref="T18:X18" si="9" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T9,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;C&lt;/td&gt;</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Hamilton BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;Napier BHS&lt;/td&gt;</v>
+      </c>
+      <c r="X18" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;HBHS 1&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -3932,8 +4633,36 @@
       <c r="Q19" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S19" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;15&lt;/td&gt;</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" ref="T19:X19" si="10" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T10,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;A&lt;/td&gt;</v>
+      </c>
+      <c r="U19" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Christchurch BHS&lt;/td&gt;</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;Wellington College&lt;/td&gt;</v>
+      </c>
+      <c r="X19" t="str">
+        <f t="shared" si="10"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y19" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;UNI 1&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
@@ -3957,8 +4686,36 @@
       <c r="Q20" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="S20" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;tr&gt;&lt;td&gt;16&lt;/td&gt;</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" ref="T20:X20" si="11" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",T11,"&lt;/td&gt;")</f>
+        <v>&lt;td&gt;A&lt;/td&gt;</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;td class='teamLeft'&gt;Tauranga Boys College&lt;/td&gt;</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;td&gt;V&lt;/td&gt;</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;td class='teamRight'&gt;Wesley College&lt;/td&gt;</v>
+      </c>
+      <c r="X20" t="str">
+        <f t="shared" si="11"/>
+        <v>&lt;td&gt;2.30pm&lt;/td&gt;</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;td&gt;UNI 2&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
@@ -3983,7 +4740,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -4008,7 +4765,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
@@ -4039,7 +4796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
@@ -4064,7 +4821,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4089,7 +4846,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
@@ -4117,7 +4874,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
@@ -4142,7 +4899,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
@@ -4167,7 +4924,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
@@ -4189,7 +4946,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:25" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
@@ -4211,7 +4968,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
@@ -4233,7 +4990,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K32" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q12, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -4421,8 +5178,8 @@
         <f t="array" ref="L41">INDEX(K$6:K$107,ROWS(K41:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
       </c>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K42" t="str">
@@ -4433,8 +5190,6 @@
         <f t="array" ref="L42">INDEX(K$6:K$107,ROWS(K42:K$107))</f>
         <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -4448,8 +5203,6 @@
         <f t="array" ref="L43">INDEX(K$6:K$107,ROWS(K43:K$107))</f>
         <v>&lt;td&gt;Final 15-0 &lt;/td&gt;</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
@@ -4463,8 +5216,6 @@
         <f t="array" ref="L44">INDEX(K$6:K$107,ROWS(K44:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
       </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
     </row>
     <row r="45" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -4700,8 +5451,8 @@
         <f t="array" ref="L60">INDEX(K$6:K$107,ROWS(K60:K$107))</f>
         <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="M60" s="13"/>
-      <c r="N60" s="13"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
@@ -4715,8 +5466,6 @@
         <f t="array" ref="L61">INDEX(K$6:K$107,ROWS(K61:K$107))</f>
         <v>&lt;td&gt;Final 18-7 &lt;/td&gt;</v>
       </c>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K62" t="str">
@@ -4727,8 +5476,6 @@
         <f t="array" ref="L62">INDEX(K$6:K$107,ROWS(K62:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
       </c>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -4742,8 +5489,6 @@
         <f t="array" ref="L63">INDEX(K$6:K$107,ROWS(K63:K$107))</f>
         <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="M63" s="11"/>
-      <c r="N63" s="11"/>
     </row>
     <row r="64" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -4979,8 +5724,8 @@
         <f t="array" ref="L79">INDEX(K$6:K$107,ROWS(K79:K$107))</f>
         <v>&lt;td&gt;Final 26-0 &lt;/td&gt;</v>
       </c>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
@@ -4994,8 +5739,6 @@
         <f t="array" ref="L80">INDEX(K$6:K$107,ROWS(K80:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
       </c>
-      <c r="M80" s="11"/>
-      <c r="N80" s="11"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -5009,8 +5752,6 @@
         <f t="array" ref="L81">INDEX(K$6:K$107,ROWS(K81:K$107))</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="M81" s="11"/>
-      <c r="N81" s="11"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K82" t="str">
@@ -5021,8 +5762,6 @@
         <f t="array" ref="L82">INDEX(K$6:K$107,ROWS(K82:K$107))</f>
         <v>&lt;td&gt;Final 20-0 &lt;/td&gt;</v>
       </c>
-      <c r="M82" s="11"/>
-      <c r="N82" s="11"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K83" t="str">
@@ -5033,8 +5772,6 @@
         <f t="array" ref="L83">INDEX(K$6:K$107,ROWS(K83:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
       </c>
-      <c r="M83" s="11"/>
-      <c r="N83" s="11"/>
     </row>
     <row r="84" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K84" t="str">
@@ -5237,8 +5974,6 @@
         <f t="array" ref="L100">INDEX(K$6:K$107,ROWS(K100:K$107))</f>
         <v>&lt;td&gt;Final 12-3 &lt;/td&gt;</v>
       </c>
-      <c r="M100" s="11"/>
-      <c r="N100" s="11"/>
     </row>
     <row r="101" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K101" t="str">
@@ -5249,8 +5984,6 @@
         <f t="array" ref="L101">INDEX(K$6:K$107,ROWS(K101:K$107))</f>
         <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
       </c>
-      <c r="M101" s="11"/>
-      <c r="N101" s="11"/>
     </row>
     <row r="102" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K102" t="str">
@@ -5261,8 +5994,6 @@
         <f t="array" ref="L102">INDEX(K$6:K$107,ROWS(K102:K$107))</f>
         <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="M102" s="11"/>
-      <c r="N102" s="11"/>
     </row>
     <row r="103" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K103" t="str">
@@ -5375,404 +6106,96 @@
       <c r="N117" s="10"/>
     </row>
     <row r="118" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L118" s="12"/>
-      <c r="M118" s="12"/>
+      <c r="L118" s="11"/>
+      <c r="M118" s="11"/>
       <c r="N118" s="10"/>
     </row>
     <row r="119" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L119" s="11"/>
-      <c r="M119" s="14"/>
-      <c r="N119" s="14"/>
+      <c r="M119" s="13"/>
+      <c r="N119" s="13"/>
     </row>
     <row r="120" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L120" s="11"/>
-      <c r="M120" s="14"/>
-      <c r="N120" s="14"/>
+      <c r="M120" s="13"/>
+      <c r="N120" s="13"/>
     </row>
     <row r="121" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L121" s="11"/>
-      <c r="M121" s="14"/>
-      <c r="N121" s="14"/>
+      <c r="M121" s="13"/>
+      <c r="N121" s="13"/>
     </row>
     <row r="122" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L122" s="10"/>
-      <c r="M122" s="14"/>
-      <c r="N122" s="14"/>
+      <c r="M122" s="13"/>
+      <c r="N122" s="13"/>
     </row>
     <row r="123" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L123" s="10"/>
-      <c r="M123" s="14"/>
-      <c r="N123" s="14"/>
+      <c r="M123" s="13"/>
+      <c r="N123" s="13"/>
     </row>
     <row r="124" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L124" s="10"/>
-      <c r="M124" s="14"/>
-      <c r="N124" s="14"/>
+      <c r="M124" s="13"/>
+      <c r="N124" s="13"/>
     </row>
     <row r="125" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L125" s="10"/>
-      <c r="M125" s="14"/>
-      <c r="N125" s="14"/>
+      <c r="M125" s="13"/>
+      <c r="N125" s="13"/>
     </row>
     <row r="126" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L126" s="10"/>
-      <c r="M126" s="14"/>
-      <c r="N126" s="14"/>
+      <c r="M126" s="13"/>
+      <c r="N126" s="13"/>
     </row>
     <row r="127" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L127" s="10"/>
-      <c r="M127" s="14"/>
-      <c r="N127" s="14"/>
+      <c r="M127" s="13"/>
+      <c r="N127" s="13"/>
     </row>
     <row r="128" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L128" s="10"/>
-      <c r="M128" s="14"/>
-      <c r="N128" s="14"/>
+      <c r="M128" s="13"/>
+      <c r="N128" s="13"/>
     </row>
     <row r="129" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L129" s="10"/>
-      <c r="M129" s="14"/>
-      <c r="N129" s="14"/>
+      <c r="M129" s="13"/>
+      <c r="N129" s="13"/>
     </row>
     <row r="130" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L130" s="10"/>
-      <c r="M130" s="14"/>
-      <c r="N130" s="14"/>
+      <c r="M130" s="13"/>
+      <c r="N130" s="13"/>
     </row>
     <row r="131" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L131" s="10"/>
-      <c r="M131" s="14"/>
-      <c r="N131" s="14"/>
+      <c r="M131" s="13"/>
+      <c r="N131" s="13"/>
     </row>
     <row r="132" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L132" s="10"/>
-      <c r="M132" s="14"/>
-      <c r="N132" s="14"/>
+      <c r="M132" s="13"/>
+      <c r="N132" s="13"/>
     </row>
     <row r="133" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L133" s="10"/>
-      <c r="M133" s="14"/>
-      <c r="N133" s="14"/>
+      <c r="M133" s="13"/>
+      <c r="N133" s="13"/>
     </row>
     <row r="134" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L134" s="10"/>
-      <c r="M134" s="14"/>
-      <c r="N134" s="14"/>
+      <c r="M134" s="13"/>
+      <c r="N134" s="13"/>
     </row>
     <row r="135" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L135" s="10"/>
-      <c r="M135" s="14"/>
-      <c r="N135" s="14"/>
+      <c r="M135" s="13"/>
+      <c r="N135" s="13"/>
     </row>
     <row r="136" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L136" s="10"/>
-      <c r="M136" s="14"/>
-      <c r="N136" s="14"/>
-    </row>
-    <row r="137" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L137" s="11"/>
-      <c r="M137" s="11"/>
-      <c r="N137" s="11"/>
-    </row>
-    <row r="138" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L138" s="11"/>
-      <c r="M138" s="11"/>
-      <c r="N138" s="11"/>
-    </row>
-    <row r="139" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L139" s="11"/>
-      <c r="M139" s="11"/>
-      <c r="N139" s="11"/>
-    </row>
-    <row r="140" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L140" s="11"/>
-      <c r="M140" s="11"/>
-      <c r="N140" s="11"/>
-    </row>
-    <row r="141" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L141" s="11"/>
-      <c r="M141" s="11"/>
-      <c r="N141" s="11"/>
-    </row>
-    <row r="142" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L142" s="11"/>
-      <c r="M142" s="11"/>
-      <c r="N142" s="11"/>
-    </row>
-    <row r="143" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L143" s="11"/>
-      <c r="M143" s="11"/>
-      <c r="N143" s="11"/>
-    </row>
-    <row r="144" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L144" s="11"/>
-      <c r="M144" s="11"/>
-      <c r="N144" s="11"/>
-    </row>
-    <row r="145" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L145" s="11"/>
-      <c r="M145" s="11"/>
-      <c r="N145" s="11"/>
-    </row>
-    <row r="146" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L146" s="11"/>
-      <c r="M146" s="11"/>
-      <c r="N146" s="11"/>
-    </row>
-    <row r="147" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L147" s="11"/>
-      <c r="M147" s="11"/>
-      <c r="N147" s="11"/>
-    </row>
-    <row r="148" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L148" s="11"/>
-      <c r="M148" s="11"/>
-      <c r="N148" s="11"/>
-    </row>
-    <row r="149" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L149" s="11"/>
-      <c r="M149" s="11"/>
-      <c r="N149" s="11"/>
-    </row>
-    <row r="150" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L150" s="11"/>
-      <c r="M150" s="11"/>
-      <c r="N150" s="11"/>
-    </row>
-    <row r="151" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L151" s="11"/>
-      <c r="M151" s="11"/>
-      <c r="N151" s="11"/>
-    </row>
-    <row r="152" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L152" s="11"/>
-      <c r="M152" s="11"/>
-      <c r="N152" s="11"/>
-    </row>
-    <row r="153" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L153" s="11"/>
-      <c r="M153" s="11"/>
-      <c r="N153" s="11"/>
-    </row>
-    <row r="154" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L154" s="11"/>
-      <c r="M154" s="11"/>
-      <c r="N154" s="11"/>
-    </row>
-    <row r="155" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L155" s="11"/>
-      <c r="M155" s="11"/>
-      <c r="N155" s="11"/>
-    </row>
-    <row r="156" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L156" s="11"/>
-      <c r="M156" s="11"/>
-      <c r="N156" s="11"/>
-    </row>
-    <row r="157" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L157" s="11"/>
-      <c r="M157" s="11"/>
-      <c r="N157" s="11"/>
-    </row>
-    <row r="158" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L158" s="11"/>
-      <c r="M158" s="11"/>
-      <c r="N158" s="11"/>
-    </row>
-    <row r="159" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L159" s="11"/>
-      <c r="M159" s="11"/>
-      <c r="N159" s="11"/>
-    </row>
-    <row r="160" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L160" s="11"/>
-      <c r="M160" s="11"/>
-      <c r="N160" s="11"/>
-    </row>
-    <row r="161" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L161" s="11"/>
-      <c r="M161" s="11"/>
-      <c r="N161" s="11"/>
-    </row>
-    <row r="162" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L162" s="11"/>
-      <c r="M162" s="11"/>
-      <c r="N162" s="11"/>
-    </row>
-    <row r="163" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L163" s="11"/>
-      <c r="M163" s="11"/>
-      <c r="N163" s="11"/>
-    </row>
-    <row r="164" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L164" s="11"/>
-      <c r="M164" s="11"/>
-      <c r="N164" s="11"/>
-    </row>
-    <row r="165" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L165" s="11"/>
-      <c r="M165" s="11"/>
-      <c r="N165" s="11"/>
-    </row>
-    <row r="166" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L166" s="11"/>
-      <c r="M166" s="11"/>
-      <c r="N166" s="11"/>
-    </row>
-    <row r="167" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L167" s="11"/>
-      <c r="M167" s="11"/>
-      <c r="N167" s="11"/>
-    </row>
-    <row r="168" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L168" s="11"/>
-      <c r="M168" s="11"/>
-      <c r="N168" s="11"/>
-    </row>
-    <row r="169" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L169" s="11"/>
-      <c r="M169" s="11"/>
-      <c r="N169" s="11"/>
-    </row>
-    <row r="170" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L170" s="11"/>
-      <c r="M170" s="11"/>
-      <c r="N170" s="11"/>
-    </row>
-    <row r="171" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L171" s="11"/>
-      <c r="M171" s="11"/>
-      <c r="N171" s="11"/>
-    </row>
-    <row r="172" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L172" s="11"/>
-      <c r="M172" s="11"/>
-      <c r="N172" s="11"/>
-    </row>
-    <row r="173" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L173" s="11"/>
-      <c r="M173" s="11"/>
-      <c r="N173" s="11"/>
-    </row>
-    <row r="174" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L174" s="11"/>
-      <c r="M174" s="11"/>
-      <c r="N174" s="11"/>
-    </row>
-    <row r="175" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L175" s="11"/>
-      <c r="M175" s="11"/>
-      <c r="N175" s="11"/>
-    </row>
-    <row r="176" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L176" s="11"/>
-      <c r="M176" s="11"/>
-      <c r="N176" s="11"/>
-    </row>
-    <row r="177" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L177" s="11"/>
-      <c r="M177" s="11"/>
-      <c r="N177" s="11"/>
-    </row>
-    <row r="178" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L178" s="11"/>
-      <c r="M178" s="11"/>
-      <c r="N178" s="11"/>
-    </row>
-    <row r="179" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L179" s="11"/>
-      <c r="M179" s="11"/>
-      <c r="N179" s="11"/>
-    </row>
-    <row r="180" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L180" s="11"/>
-      <c r="M180" s="11"/>
-      <c r="N180" s="11"/>
-    </row>
-    <row r="181" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L181" s="11"/>
-      <c r="M181" s="11"/>
-      <c r="N181" s="11"/>
-    </row>
-    <row r="182" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L182" s="11"/>
-      <c r="M182" s="11"/>
-      <c r="N182" s="11"/>
-    </row>
-    <row r="183" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L183" s="11"/>
-      <c r="M183" s="11"/>
-      <c r="N183" s="11"/>
-    </row>
-    <row r="184" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L184" s="11"/>
-      <c r="M184" s="11"/>
-      <c r="N184" s="11"/>
-    </row>
-    <row r="185" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L185" s="11"/>
-      <c r="M185" s="11"/>
-      <c r="N185" s="11"/>
-    </row>
-    <row r="186" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L186" s="11"/>
-      <c r="M186" s="11"/>
-      <c r="N186" s="11"/>
-    </row>
-    <row r="187" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L187" s="11"/>
-      <c r="M187" s="11"/>
-      <c r="N187" s="11"/>
-    </row>
-    <row r="188" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L188" s="11"/>
-      <c r="M188" s="11"/>
-      <c r="N188" s="11"/>
-    </row>
-    <row r="189" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L189" s="11"/>
-      <c r="M189" s="11"/>
-      <c r="N189" s="11"/>
-    </row>
-    <row r="190" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L190" s="11"/>
-      <c r="M190" s="11"/>
-      <c r="N190" s="11"/>
-    </row>
-    <row r="191" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L191" s="11"/>
-      <c r="M191" s="11"/>
-      <c r="N191" s="11"/>
-    </row>
-    <row r="192" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L192" s="11"/>
-      <c r="M192" s="11"/>
-      <c r="N192" s="11"/>
-    </row>
-    <row r="193" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L193" s="11"/>
-      <c r="M193" s="11"/>
-      <c r="N193" s="11"/>
-    </row>
-    <row r="194" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L194" s="11"/>
-      <c r="M194" s="11"/>
-      <c r="N194" s="11"/>
-    </row>
-    <row r="195" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L195" s="11"/>
-      <c r="M195" s="11"/>
-      <c r="N195" s="11"/>
-    </row>
-    <row r="196" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L196" s="11"/>
-      <c r="M196" s="11"/>
-      <c r="N196" s="11"/>
-    </row>
-    <row r="197" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="L197" s="11"/>
-      <c r="M197" s="11"/>
-      <c r="N197" s="11"/>
+      <c r="M136" s="13"/>
+      <c r="N136" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
flipping the table upside down
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\13IA\Project\13IA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{1B07BBE5-48F2-45D5-82CD-7670E775B07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6ACE38-6804-48F7-A265-138722ED4978}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FC1D6-A3EB-4960-94DC-D9EF11929F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2670" windowWidth="29040" windowHeight="15840" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3509,9 +3487,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3571,6 +3546,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3586,10 +3564,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3891,16 +3865,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD87F2E1-A52F-4456-AB4D-EECF95DE5FBF}">
   <dimension ref="B3:Y136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:Y20"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52:K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.140625" customWidth="1"/>
@@ -3930,25 +3905,25 @@
       <c r="Q4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="13">
         <v>9</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="V4" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="W4" s="16" t="s">
+      <c r="W4" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="X4" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="Y4" s="18" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3971,25 +3946,25 @@
       <c r="Q5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="S5" s="14">
+      <c r="S5" s="13">
         <v>10</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="U5" s="16" t="s">
+      <c r="U5" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="W5" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="Y5" s="19" t="s">
+      <c r="Y5" s="18" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4003,14 +3978,6 @@
       <c r="H6" t="s">
         <v>67</v>
       </c>
-      <c r="K6" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O4, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1985 &lt;/td&gt;</v>
-      </c>
-      <c r="L6" t="str" cm="1">
-        <f t="array" ref="L6">INDEX(K$6:K$107,ROWS(K6:K$107))</f>
-        <v>&lt;td&gt;1. Hamilton BHS&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O6" s="6" t="s">
         <v>72</v>
       </c>
@@ -4020,25 +3987,25 @@
       <c r="Q6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="13">
         <v>11</v>
       </c>
-      <c r="T6" s="21" t="s">
+      <c r="T6" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="U6" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="V6" s="23" t="s">
+      <c r="V6" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="W6" s="16" t="s">
+      <c r="W6" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="X6" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="Y6" s="19" t="s">
+      <c r="Y6" s="18" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4049,14 +4016,6 @@
       <c r="H7" t="s">
         <v>68</v>
       </c>
-      <c r="K7" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O5, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L7" t="str" cm="1">
-        <f t="array" ref="L7">INDEX(K$6:K$107,ROWS(K7:K$107))</f>
-        <v>&lt;td&gt;Final 17-21&lt;/td&gt;</v>
-      </c>
       <c r="O7" s="5" t="s">
         <v>78</v>
       </c>
@@ -4066,25 +4025,25 @@
       <c r="Q7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S7" s="13">
         <v>12</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="V7" s="14" t="s">
+      <c r="V7" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="W7" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="X7" s="25" t="s">
+      <c r="X7" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="Y7" s="26" t="s">
+      <c r="Y7" s="25" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4095,14 +4054,6 @@
       <c r="H8" t="s">
         <v>69</v>
       </c>
-      <c r="K8" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O6, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L8" t="str" cm="1">
-        <f t="array" ref="L8">INDEX(K$6:K$107,ROWS(K8:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland Grammar 2018&lt;/td&gt;</v>
-      </c>
       <c r="O8" s="5" t="s">
         <v>79</v>
       </c>
@@ -4112,25 +4063,25 @@
       <c r="Q8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="S8" s="27">
+      <c r="S8" s="26">
         <v>13</v>
       </c>
-      <c r="T8" s="28" t="s">
+      <c r="T8" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="U8" s="29" t="s">
+      <c r="U8" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="V8" s="30" t="s">
+      <c r="V8" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="W8" s="16" t="s">
+      <c r="W8" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="X8" s="25" t="s">
+      <c r="X8" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="Y8" s="31" t="s">
+      <c r="Y8" s="30" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4138,14 +4089,6 @@
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P4, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1986 &lt;/td&gt;</v>
-      </c>
-      <c r="L9" t="str" cm="1">
-        <f t="array" ref="L9">INDEX(K$6:K$107,ROWS(K9:K$107))</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O9" s="6" t="s">
         <v>80</v>
       </c>
@@ -4155,25 +4098,25 @@
       <c r="Q9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S9" s="27">
+      <c r="S9" s="26">
         <v>14</v>
       </c>
-      <c r="T9" s="32" t="s">
+      <c r="T9" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="U9" s="33" t="s">
+      <c r="U9" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="V9" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="W9" s="34" t="s">
+      <c r="W9" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="X9" s="25" t="s">
+      <c r="X9" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="Y9" s="35" t="s">
+      <c r="Y9" s="34" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4184,14 +4127,6 @@
       <c r="E10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K10" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P5, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 8-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L10" t="str" cm="1">
-        <f t="array" ref="L10">INDEX(K$6:K$107,ROWS(K10:K$107))</f>
-        <v>&lt;td&gt;Final 22-18 &lt;/td&gt;</v>
-      </c>
       <c r="O10" s="5" t="s">
         <v>85</v>
       </c>
@@ -4201,25 +4136,25 @@
       <c r="Q10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="S10" s="14">
+      <c r="S10" s="13">
         <v>15</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="T10" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="U10" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="V10" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="W10" s="36" t="s">
+      <c r="W10" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="X10" s="25" t="s">
+      <c r="X10" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="Y10" s="35" t="s">
+      <c r="Y10" s="34" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4230,14 +4165,6 @@
       <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="K11" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P6, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L11" t="str" cm="1">
-        <f t="array" ref="L11">INDEX(K$6:K$107,ROWS(K11:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2017 &lt;/td&gt;</v>
-      </c>
       <c r="O11" s="5" t="s">
         <v>86</v>
       </c>
@@ -4247,25 +4174,25 @@
       <c r="Q11" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="S11" s="27">
+      <c r="S11" s="26">
         <v>16</v>
       </c>
-      <c r="T11" s="32" t="s">
+      <c r="T11" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="V11" s="28" t="s">
+      <c r="V11" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="W11" s="24" t="s">
+      <c r="W11" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="X11" s="25" t="s">
+      <c r="X11" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="Y11" s="35" t="s">
+      <c r="Y11" s="34" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4276,14 +4203,6 @@
       <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="K12" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q4, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
-      </c>
-      <c r="L12" t="str" cm="1">
-        <f t="array" ref="L12">INDEX(K$6:K$107,ROWS(K12:K$107))</f>
-        <v>&lt;td&gt;1.Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O12" s="6" t="s">
         <v>72</v>
       </c>
@@ -4301,14 +4220,6 @@
       <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="K13" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q5, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 12-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L13" t="str" cm="1">
-        <f t="array" ref="L13">INDEX(K$6:K$107,ROWS(K13:K$107))</f>
-        <v>&lt;td&gt;Final &lt;/td&gt;</v>
-      </c>
       <c r="O13" s="4" t="s">
         <v>92</v>
       </c>
@@ -4331,7 +4242,7 @@
         <v>&lt;td class='teamLeft'&gt;Auckland Grammar School&lt;/td&gt;</v>
       </c>
       <c r="V13" t="str">
-        <f t="shared" ref="U13:Y13" si="0" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",V4,"&lt;/td&gt;")</f>
+        <f t="shared" ref="V13:X13" si="0" xml:space="preserve"> _xlfn.CONCAT("&lt;td&gt;",V4,"&lt;/td&gt;")</f>
         <v>&lt;td&gt;V&lt;/td&gt;</v>
       </c>
       <c r="W13" t="str">
@@ -4351,14 +4262,6 @@
       <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="K14" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q6, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L14" t="str" cm="1">
-        <f t="array" ref="L14">INDEX(K$6:K$107,ROWS(K14:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Massey High School 2016 &lt;/td&gt;</v>
-      </c>
       <c r="O14" s="5" t="s">
         <v>93</v>
       </c>
@@ -4404,14 +4307,6 @@
       <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="K15" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O7, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>
-      </c>
-      <c r="L15" t="str" cm="1">
-        <f t="array" ref="L15">INDEX(K$6:K$107,ROWS(K15:K$107))</f>
-        <v>&lt;td&gt;1.Wesley College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O15" s="6" t="s">
         <v>72</v>
       </c>
@@ -4457,14 +4352,6 @@
       <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="K16" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O8, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 17-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L16" t="str" cm="1">
-        <f t="array" ref="L16">INDEX(K$6:K$107,ROWS(K16:K$107))</f>
-        <v>&lt;td&gt;Final &lt;/td&gt;</v>
-      </c>
       <c r="O16" s="5" t="s">
         <v>98</v>
       </c>
@@ -4510,14 +4397,6 @@
       <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="K17" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O9, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L17" t="str" cm="1">
-        <f t="array" ref="L17">INDEX(K$6:K$107,ROWS(K17:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2015 &lt;/td&gt;</v>
-      </c>
       <c r="O17" s="5" t="s">
         <v>99</v>
       </c>
@@ -4563,14 +4442,6 @@
       <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="K18" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P7, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
-      </c>
-      <c r="L18" t="str" cm="1">
-        <f t="array" ref="L18">INDEX(K$6:K$107,ROWS(K18:K$107))</f>
-        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O18" s="6" t="s">
         <v>72</v>
       </c>
@@ -4616,14 +4487,6 @@
       <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="K19" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P8, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 6-4 &lt;/td&gt;</v>
-      </c>
-      <c r="L19" t="str" cm="1">
-        <f t="array" ref="L19">INDEX(K$6:K$107,ROWS(K19:K$107))</f>
-        <v>&lt;td&gt;Final 27-26 &lt;/td&gt;</v>
-      </c>
       <c r="O19" s="5" t="s">
         <v>105</v>
       </c>
@@ -4669,14 +4532,6 @@
       <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="K20" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P9, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L20" t="str" cm="1">
-        <f t="array" ref="L20">INDEX(K$6:K$107,ROWS(K20:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2014 &lt;/td&gt;</v>
-      </c>
       <c r="O20" s="5" t="s">
         <v>106</v>
       </c>
@@ -4722,14 +4577,6 @@
       <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="K21" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q7, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
-      </c>
-      <c r="L21" t="str" cm="1">
-        <f t="array" ref="L21">INDEX(K$6:K$107,ROWS(K21:K$107))</f>
-        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O21" s="6" t="s">
         <v>107</v>
       </c>
@@ -4747,14 +4594,6 @@
       <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="K22" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q8, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 12-0 &lt;/td&gt;</v>
-      </c>
-      <c r="L22" t="str" cm="1">
-        <f t="array" ref="L22">INDEX(K$6:K$107,ROWS(K22:K$107))</f>
-        <v>&lt;td&gt;Final 14-7 &lt;/td&gt;</v>
-      </c>
       <c r="O22" s="5" t="s">
         <v>112</v>
       </c>
@@ -4778,14 +4617,6 @@
       <c r="G23" t="s">
         <v>58</v>
       </c>
-      <c r="K23" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q9, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L23" t="str" cm="1">
-        <f t="array" ref="L23">INDEX(K$6:K$107,ROWS(K23:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 2013 &lt;/td&gt;</v>
-      </c>
       <c r="O23" s="5" t="s">
         <v>113</v>
       </c>
@@ -4803,14 +4634,6 @@
       <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="K24" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O10, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
-      </c>
-      <c r="L24" t="str" cm="1">
-        <f t="array" ref="L24">INDEX(K$6:K$107,ROWS(K24:K$107))</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O24" s="6" t="s">
         <v>75</v>
       </c>
@@ -4828,14 +4651,6 @@
       <c r="E25" t="s">
         <v>62</v>
       </c>
-      <c r="K25" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O11, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 18-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L25" t="str" cm="1">
-        <f t="array" ref="L25">INDEX(K$6:K$107,ROWS(K25:K$107))</f>
-        <v>&lt;td&gt;Final 38-10 &lt;/td&gt;</v>
-      </c>
       <c r="O25" s="5" t="s">
         <v>119</v>
       </c>
@@ -4856,14 +4671,6 @@
       <c r="F26" t="s">
         <v>64</v>
       </c>
-      <c r="K26" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O12, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L26" t="str" cm="1">
-        <f t="array" ref="L26">INDEX(K$6:K$107,ROWS(K26:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Rotorua 2012 &lt;/td&gt;</v>
-      </c>
       <c r="O26" s="5" t="s">
         <v>120</v>
       </c>
@@ -4881,14 +4688,6 @@
       <c r="E27" t="s">
         <v>63</v>
       </c>
-      <c r="K27" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P10, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
-      </c>
-      <c r="L27" t="str" cm="1">
-        <f t="array" ref="L27">INDEX(K$6:K$107,ROWS(K27:K$107))</f>
-        <v>&lt;td&gt;1. Tauranga Boys’ College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O27" s="6" t="s">
         <v>121</v>
       </c>
@@ -4899,20 +4698,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E28" t="s">
         <v>59</v>
-      </c>
-      <c r="K28" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P11, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 9-6 &lt;/td&gt;</v>
-      </c>
-      <c r="L28" t="str" cm="1">
-        <f t="array" ref="L28">INDEX(K$6:K$107,ROWS(K28:K$107))</f>
-        <v>&lt;td&gt;Final 10-7 &lt;/td&gt;</v>
       </c>
       <c r="O28" s="5" t="s">
         <v>127</v>
@@ -4928,14 +4719,6 @@
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K29" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P12, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L29" t="str" cm="1">
-        <f t="array" ref="L29">INDEX(K$6:K$107,ROWS(K29:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hastings 2011 &lt;/td&gt;</v>
-      </c>
       <c r="O29" s="5" t="s">
         <v>128</v>
       </c>
@@ -4946,18 +4729,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="2:25" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K30" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q10, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
-      </c>
-      <c r="L30" t="str" cm="1">
-        <f t="array" ref="L30">INDEX(K$6:K$107,ROWS(K30:K$107))</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O30" s="6" t="s">
         <v>89</v>
       </c>
@@ -4968,18 +4743,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="2:25" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K31" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q11, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 20-0 &lt;/td&gt;</v>
-      </c>
-      <c r="L31" t="str" cm="1">
-        <f t="array" ref="L31">INDEX(K$6:K$107,ROWS(K31:K$107))</f>
-        <v>&lt;td&gt;Final 14-6 &lt;/td&gt;</v>
-      </c>
       <c r="O31" s="4" t="s">
         <v>134</v>
       </c>
@@ -4991,14 +4758,6 @@
       </c>
     </row>
     <row r="32" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K32" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q12, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L32" t="str" cm="1">
-        <f t="array" ref="L32">INDEX(K$6:K$107,ROWS(K32:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;St Bede’s 2010 &lt;/td&gt;</v>
-      </c>
       <c r="O32" s="5" t="s">
         <v>135</v>
       </c>
@@ -5009,18 +4768,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K33" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O13, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
-      </c>
-      <c r="L33" t="str" cm="1">
-        <f t="array" ref="L33">INDEX(K$6:K$107,ROWS(K33:K$107))</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O33" s="6" t="s">
         <v>89</v>
       </c>
@@ -5031,17 +4782,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="K34" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O14, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 26-0 &lt;/td&gt;</v>
-      </c>
-      <c r="L34" t="str" cm="1">
-        <f t="array" ref="L34">INDEX(K$6:K$107,ROWS(K34:K$107))</f>
-        <v>&lt;td&gt;Final 24-5 &lt;/td&gt;</v>
       </c>
       <c r="O34" s="5" t="s">
         <v>141</v>
@@ -5057,14 +4800,6 @@
       <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K35" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O15, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L35" t="str" cm="1">
-        <f t="array" ref="L35">INDEX(K$6:K$107,ROWS(K35:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;New Plymouth 2009 &lt;/td&gt;</v>
-      </c>
       <c r="O35" s="5" t="s">
         <v>142</v>
       </c>
@@ -5075,18 +4810,10 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K36" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P13, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
-      </c>
-      <c r="L36" t="str" cm="1">
-        <f t="array" ref="L36">INDEX(K$6:K$107,ROWS(K36:K$107))</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O36" s="6" t="s">
         <v>143</v>
       </c>
@@ -5097,17 +4824,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="K37" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P14, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 9-5 &lt;/td&gt;</v>
-      </c>
-      <c r="L37" t="str" cm="1">
-        <f t="array" ref="L37">INDEX(K$6:K$107,ROWS(K37:K$107))</f>
-        <v>&lt;td&gt;Final 20-3 &lt;/td&gt;</v>
       </c>
       <c r="O37" s="5" t="s">
         <v>148</v>
@@ -5119,14 +4838,6 @@
       <c r="B38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K38" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P15, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L38" t="str" cm="1">
-        <f t="array" ref="L38">INDEX(K$6:K$107,ROWS(K38:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2008 &lt;/td&gt;</v>
-      </c>
       <c r="O38" s="5" t="s">
         <v>149</v>
       </c>
@@ -5137,14 +4848,6 @@
       <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K39" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q13, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
-      </c>
-      <c r="L39" t="str" cm="1">
-        <f t="array" ref="L39">INDEX(K$6:K$107,ROWS(K39:K$107))</f>
-        <v>&lt;td&gt;1. Palmerston North BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="O39" s="6" t="s">
         <v>150</v>
       </c>
@@ -5155,14 +4858,6 @@
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K40" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q14, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 22-5 &lt;/td&gt;</v>
-      </c>
-      <c r="L40" t="str" cm="1">
-        <f t="array" ref="L40">INDEX(K$6:K$107,ROWS(K40:K$107))</f>
-        <v>&lt;td&gt;Final 18-15 &lt;/td&gt;</v>
-      </c>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
@@ -5170,65 +4865,23 @@
       <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K41" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q15, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L41" t="str" cm="1">
-        <f t="array" ref="L41">INDEX(K$6:K$107,ROWS(K41:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
-      </c>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K42" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O16, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
-      </c>
-      <c r="L42" t="str" cm="1">
-        <f t="array" ref="L42">INDEX(K$6:K$107,ROWS(K42:K$107))</f>
-        <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K43" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O17, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 16-13 &lt;/td&gt;</v>
-      </c>
-      <c r="L43" t="str" cm="1">
-        <f t="array" ref="L43">INDEX(K$6:K$107,ROWS(K43:K$107))</f>
-        <v>&lt;td&gt;Final 15-0 &lt;/td&gt;</v>
-      </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K44" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O18, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L44" t="str" cm="1">
-        <f t="array" ref="L44">INDEX(K$6:K$107,ROWS(K44:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
-      </c>
     </row>
     <row r="45" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K45" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P16, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
-      </c>
-      <c r="L45" t="str" cm="1">
-        <f t="array" ref="L45">INDEX(K$6:K$107,ROWS(K45:K$107))</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
     </row>
@@ -5236,14 +4889,6 @@
       <c r="B46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K46" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P17, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 14-13 &lt;/td&gt;</v>
-      </c>
-      <c r="L46" t="str" cm="1">
-        <f t="array" ref="L46">INDEX(K$6:K$107,ROWS(K46:K$107))</f>
-        <v>&lt;td&gt;Final 20-12 &lt;/td&gt;</v>
-      </c>
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
     </row>
@@ -5251,14 +4896,6 @@
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K47" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P18, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L47" t="str" cm="1">
-        <f t="array" ref="L47">INDEX(K$6:K$107,ROWS(K47:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 2005 &lt;/td&gt;</v>
-      </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
     </row>
@@ -5266,14 +4903,6 @@
       <c r="B48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K48" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q16, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
-      </c>
-      <c r="L48" t="str" cm="1">
-        <f t="array" ref="L48">INDEX(K$6:K$107,ROWS(K48:K$107))</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
     </row>
@@ -5281,14 +4910,6 @@
       <c r="B49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K49" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q17, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 13-12 &lt;/td&gt;</v>
-      </c>
-      <c r="L49" t="str" cm="1">
-        <f t="array" ref="L49">INDEX(K$6:K$107,ROWS(K49:K$107))</f>
-        <v>&lt;td&gt;Final 47-0 &lt;/td&gt;</v>
-      </c>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
     </row>
@@ -5296,14 +4917,6 @@
       <c r="B50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K50" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q18, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L50" t="str" cm="1">
-        <f t="array" ref="L50">INDEX(K$6:K$107,ROWS(K50:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 2004 &lt;/td&gt;</v>
-      </c>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
     </row>
@@ -5311,25 +4924,13 @@
       <c r="B51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K51" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O19, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
-      </c>
-      <c r="L51" t="str" cm="1">
-        <f t="array" ref="L51">INDEX(K$6:K$107,ROWS(K51:K$107))</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
       <c r="M51" s="10"/>
       <c r="N51" s="10"/>
     </row>
     <row r="52" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K52" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O20, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 18-7 &lt;/td&gt;</v>
-      </c>
-      <c r="L52" t="str" cm="1">
-        <f t="array" ref="L52">INDEX(K$6:K$107,ROWS(K52:K$107))</f>
-        <v>&lt;td&gt;Final 22-14 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O37, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland Grammar 2018&lt;/td&gt;</v>
       </c>
       <c r="M52" s="10"/>
       <c r="N52" s="10"/>
@@ -5339,12 +4940,8 @@
         <v>10</v>
       </c>
       <c r="K53" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O21, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L53" t="str" cm="1">
-        <f t="array" ref="L53">INDEX(K$6:K$107,ROWS(K53:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 2003 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O39, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
@@ -5354,12 +4951,8 @@
         <v>6</v>
       </c>
       <c r="K54" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P19, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
-      </c>
-      <c r="L54" t="str" cm="1">
-        <f t="array" ref="L54">INDEX(K$6:K$107,ROWS(K54:K$107))</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2017 &lt;/td&gt;</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
@@ -5369,12 +4962,8 @@
         <v>13</v>
       </c>
       <c r="K55" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P20, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 27-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L55" t="str" cm="1">
-        <f t="array" ref="L55">INDEX(K$6:K$107,ROWS(K55:K$107))</f>
-        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
@@ -5384,12 +4973,8 @@
         <v>20</v>
       </c>
       <c r="K56" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P21, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L56" t="str" cm="1">
-        <f t="array" ref="L56">INDEX(K$6:K$107,ROWS(K56:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Massey High School 2016 &lt;/td&gt;</v>
       </c>
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
@@ -5399,12 +4984,8 @@
         <v>23</v>
       </c>
       <c r="K57" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q19, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
-      </c>
-      <c r="L57" t="str" cm="1">
-        <f t="array" ref="L57">INDEX(K$6:K$107,ROWS(K57:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1.Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
@@ -5414,12 +4995,8 @@
         <v>29</v>
       </c>
       <c r="K58" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q20, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L58" t="str" cm="1">
-        <f t="array" ref="L58">INDEX(K$6:K$107,ROWS(K58:K$107))</f>
-        <v>&lt;td&gt;Final 27-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O34, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2015 &lt;/td&gt;</v>
       </c>
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
@@ -5429,12 +5006,8 @@
         <v>32</v>
       </c>
       <c r="K59" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q21, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L59" t="str" cm="1">
-        <f t="array" ref="L59">INDEX(K$6:K$107,ROWS(K59:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O36, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1.Wesley College &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
@@ -5444,12 +5017,8 @@
         <v>38</v>
       </c>
       <c r="K60" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O22, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 2003 &lt;/td&gt;</v>
-      </c>
-      <c r="L60" t="str" cm="1">
-        <f t="array" ref="L60">INDEX(K$6:K$107,ROWS(K60:K$107))</f>
-        <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2014 &lt;/td&gt;</v>
       </c>
       <c r="M60" s="12"/>
       <c r="N60" s="12"/>
@@ -5459,22 +5028,14 @@
         <v>9</v>
       </c>
       <c r="K61" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O23, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 22-14 &lt;/td&gt;</v>
-      </c>
-      <c r="L61" t="str" cm="1">
-        <f t="array" ref="L61">INDEX(K$6:K$107,ROWS(K61:K$107))</f>
-        <v>&lt;td&gt;Final 18-7 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K62" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O24, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L62" t="str" cm="1">
-        <f t="array" ref="L62">INDEX(K$6:K$107,ROWS(K62:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 2013 &lt;/td&gt;</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -5482,12 +5043,8 @@
         <v>10</v>
       </c>
       <c r="K63" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P22, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 2004 &lt;/td&gt;</v>
-      </c>
-      <c r="L63" t="str" cm="1">
-        <f t="array" ref="L63">INDEX(K$6:K$107,ROWS(K63:K$107))</f>
-        <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="64" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5495,12 +5052,8 @@
         <v>7</v>
       </c>
       <c r="K64" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P23, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 47-0 &lt;/td&gt;</v>
-      </c>
-      <c r="L64" t="str" cm="1">
-        <f t="array" ref="L64">INDEX(K$6:K$107,ROWS(K64:K$107))</f>
-        <v>&lt;td&gt;Final 13-12 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O31, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Rotorua 2012 &lt;/td&gt;</v>
       </c>
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
@@ -5510,12 +5063,8 @@
         <v>14</v>
       </c>
       <c r="K65" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P24, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L65" t="str" cm="1">
-        <f t="array" ref="L65">INDEX(K$6:K$107,ROWS(K65:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O33, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
@@ -5525,12 +5074,8 @@
         <v>21</v>
       </c>
       <c r="K66" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q22, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 2005 &lt;/td&gt;</v>
-      </c>
-      <c r="L66" t="str" cm="1">
-        <f t="array" ref="L66">INDEX(K$6:K$107,ROWS(K66:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hastings 2011 &lt;/td&gt;</v>
       </c>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
@@ -5540,12 +5085,8 @@
         <v>23</v>
       </c>
       <c r="K67" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q23, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 20-12 &lt;/td&gt;</v>
-      </c>
-      <c r="L67" t="str" cm="1">
-        <f t="array" ref="L67">INDEX(K$6:K$107,ROWS(K67:K$107))</f>
-        <v>&lt;td&gt;Final 14-13 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Tauranga Boys’ College &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
@@ -5555,12 +5096,8 @@
         <v>30</v>
       </c>
       <c r="K68" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q24, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L68" t="str" cm="1">
-        <f t="array" ref="L68">INDEX(K$6:K$107,ROWS(K68:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;St Bede’s 2010 &lt;/td&gt;</v>
       </c>
       <c r="M68" s="10"/>
       <c r="N68" s="10"/>
@@ -5570,12 +5107,8 @@
         <v>32</v>
       </c>
       <c r="K69" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O25, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
-      </c>
-      <c r="L69" t="str" cm="1">
-        <f t="array" ref="L69">INDEX(K$6:K$107,ROWS(K69:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M69" s="10"/>
       <c r="N69" s="10"/>
@@ -5585,12 +5118,8 @@
         <v>39</v>
       </c>
       <c r="K70" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O26, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 15-0 &lt;/td&gt;</v>
-      </c>
-      <c r="L70" t="str" cm="1">
-        <f t="array" ref="L70">INDEX(K$6:K$107,ROWS(K70:K$107))</f>
-        <v>&lt;td&gt;Final 16-13 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O28, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;New Plymouth 2009 &lt;/td&gt;</v>
       </c>
       <c r="M70" s="10"/>
       <c r="N70" s="10"/>
@@ -5600,24 +5129,16 @@
         <v>9</v>
       </c>
       <c r="K71" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O27, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L71" t="str" cm="1">
-        <f t="array" ref="L71">INDEX(K$6:K$107,ROWS(K71:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O30, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M71" s="10"/>
       <c r="N71" s="10"/>
     </row>
     <row r="72" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K72" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P25, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
-      </c>
-      <c r="L72" t="str" cm="1">
-        <f t="array" ref="L72">INDEX(K$6:K$107,ROWS(K72:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2008 &lt;/td&gt;</v>
       </c>
       <c r="M72" s="10"/>
       <c r="N72" s="10"/>
@@ -5627,12 +5148,8 @@
         <v>10</v>
       </c>
       <c r="K73" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P26, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 18-15 &lt;/td&gt;</v>
-      </c>
-      <c r="L73" t="str" cm="1">
-        <f t="array" ref="L73">INDEX(K$6:K$107,ROWS(K73:K$107))</f>
-        <v>&lt;td&gt;Final 22-5 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M73" s="10"/>
       <c r="N73" s="10"/>
@@ -5642,12 +5159,8 @@
         <v>8</v>
       </c>
       <c r="K74" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P27, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Palmerston North BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L74" t="str" cm="1">
-        <f t="array" ref="L74">INDEX(K$6:K$107,ROWS(K74:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wesley 2007 &lt;/td&gt;</v>
       </c>
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
@@ -5657,12 +5170,8 @@
         <v>14</v>
       </c>
       <c r="K75" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q25, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2008 &lt;/td&gt;</v>
-      </c>
-      <c r="L75" t="str" cm="1">
-        <f t="array" ref="L75">INDEX(K$6:K$107,ROWS(K75:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Palmerston North BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
@@ -5672,12 +5181,8 @@
         <v>22</v>
       </c>
       <c r="K76" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q26, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 20-3 &lt;/td&gt;</v>
-      </c>
-      <c r="L76" t="str" cm="1">
-        <f t="array" ref="L76">INDEX(K$6:K$107,ROWS(K76:K$107))</f>
-        <v>&lt;td&gt;Final 9-5 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O25, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Tauranga 2006 &lt;/td&gt;</v>
       </c>
       <c r="M76" s="10"/>
       <c r="N76" s="10"/>
@@ -5687,12 +5192,8 @@
         <v>23</v>
       </c>
       <c r="K77" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q27, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L77" t="str" cm="1">
-        <f t="array" ref="L77">INDEX(K$6:K$107,ROWS(K77:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O27, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Wellington College &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
@@ -5702,12 +5203,8 @@
         <v>31</v>
       </c>
       <c r="K78" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O28, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;New Plymouth 2009 &lt;/td&gt;</v>
-      </c>
-      <c r="L78" t="str" cm="1">
-        <f t="array" ref="L78">INDEX(K$6:K$107,ROWS(K78:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 2005 &lt;/td&gt;</v>
       </c>
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
@@ -5717,12 +5214,8 @@
         <v>32</v>
       </c>
       <c r="K79" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O29, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 24-5 &lt;/td&gt;</v>
-      </c>
-      <c r="L79" t="str" cm="1">
-        <f t="array" ref="L79">INDEX(K$6:K$107,ROWS(K79:K$107))</f>
-        <v>&lt;td&gt;Final 26-0 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M79" s="12"/>
       <c r="N79" s="12"/>
@@ -5732,12 +5225,8 @@
         <v>40</v>
       </c>
       <c r="K80" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O30, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L80" t="str" cm="1">
-        <f t="array" ref="L80">INDEX(K$6:K$107,ROWS(K80:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 2004 &lt;/td&gt;</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
@@ -5745,221 +5234,145 @@
         <v>9</v>
       </c>
       <c r="K81" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P28, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;St Bede’s 2010 &lt;/td&gt;</v>
-      </c>
-      <c r="L81" t="str" cm="1">
-        <f t="array" ref="L81">INDEX(K$6:K$107,ROWS(K81:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K82" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P29, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 14-6 &lt;/td&gt;</v>
-      </c>
-      <c r="L82" t="str" cm="1">
-        <f t="array" ref="L82">INDEX(K$6:K$107,ROWS(K82:K$107))</f>
-        <v>&lt;td&gt;Final 20-0 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O22, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 2003 &lt;/td&gt;</v>
       </c>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K83" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P30, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L83" t="str" cm="1">
-        <f t="array" ref="L83">INDEX(K$6:K$107,ROWS(K83:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O24, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="84" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K84" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q28, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hastings 2011 &lt;/td&gt;</v>
-      </c>
-      <c r="L84" t="str" cm="1">
-        <f t="array" ref="L84">INDEX(K$6:K$107,ROWS(K84:K$107))</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
       </c>
       <c r="M84" s="10"/>
       <c r="N84" s="10"/>
     </row>
     <row r="85" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K85" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q29, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 10-7 &lt;/td&gt;</v>
-      </c>
-      <c r="L85" t="str" cm="1">
-        <f t="array" ref="L85">INDEX(K$6:K$107,ROWS(K85:K$107))</f>
-        <v>&lt;td&gt;Final 9-6 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M85" s="10"/>
       <c r="N85" s="10"/>
     </row>
     <row r="86" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K86" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q30, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Tauranga Boys’ College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L86" t="str" cm="1">
-        <f t="array" ref="L86">INDEX(K$6:K$107,ROWS(K86:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
       </c>
       <c r="M86" s="10"/>
       <c r="N86" s="10"/>
     </row>
     <row r="87" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K87" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O31, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Rotorua 2012 &lt;/td&gt;</v>
-      </c>
-      <c r="L87" t="str" cm="1">
-        <f t="array" ref="L87">INDEX(K$6:K$107,ROWS(K87:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M87" s="10"/>
       <c r="N87" s="10"/>
     </row>
     <row r="88" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K88" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O32, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 38-10 &lt;/td&gt;</v>
-      </c>
-      <c r="L88" t="str" cm="1">
-        <f t="array" ref="L88">INDEX(K$6:K$107,ROWS(K88:K$107))</f>
-        <v>&lt;td&gt;Final 18-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O19, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
       </c>
       <c r="M88" s="10"/>
       <c r="N88" s="10"/>
     </row>
     <row r="89" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K89" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O33, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L89" t="str" cm="1">
-        <f t="array" ref="L89">INDEX(K$6:K$107,ROWS(K89:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O21, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M89" s="10"/>
       <c r="N89" s="10"/>
     </row>
     <row r="90" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K90" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P31, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 2013 &lt;/td&gt;</v>
-      </c>
-      <c r="L90" t="str" cm="1">
-        <f t="array" ref="L90">INDEX(K$6:K$107,ROWS(K90:K$107))</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
       </c>
       <c r="M90" s="10"/>
       <c r="N90" s="10"/>
     </row>
     <row r="91" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K91" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P32, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 14-7 &lt;/td&gt;</v>
-      </c>
-      <c r="L91" t="str" cm="1">
-        <f t="array" ref="L91">INDEX(K$6:K$107,ROWS(K91:K$107))</f>
-        <v>&lt;td&gt;Final 12-0 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
     </row>
     <row r="92" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K92" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P33, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L92" t="str" cm="1">
-        <f t="array" ref="L92">INDEX(K$6:K$107,ROWS(K92:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
       </c>
       <c r="M92" s="10"/>
       <c r="N92" s="10"/>
     </row>
     <row r="93" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K93" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q31, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2014 &lt;/td&gt;</v>
-      </c>
-      <c r="L93" t="str" cm="1">
-        <f t="array" ref="L93">INDEX(K$6:K$107,ROWS(K93:K$107))</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M93" s="10"/>
       <c r="N93" s="10"/>
     </row>
     <row r="94" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K94" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q32, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 27-26 &lt;/td&gt;</v>
-      </c>
-      <c r="L94" t="str" cm="1">
-        <f t="array" ref="L94">INDEX(K$6:K$107,ROWS(K94:K$107))</f>
-        <v>&lt;td&gt;Final 6-4 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O16, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
       </c>
       <c r="M94" s="10"/>
       <c r="N94" s="10"/>
     </row>
     <row r="95" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K95" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q33, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Hamilton BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L95" t="str" cm="1">
-        <f t="array" ref="L95">INDEX(K$6:K$107,ROWS(K95:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O18, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
     </row>
     <row r="96" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K96" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O34, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Dunedin 2015 &lt;/td&gt;</v>
-      </c>
-      <c r="L96" t="str" cm="1">
-        <f t="array" ref="L96">INDEX(K$6:K$107,ROWS(K96:K$107))</f>
-        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
       </c>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
     </row>
     <row r="97" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K97" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O35, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final &lt;/td&gt;</v>
-      </c>
-      <c r="L97" t="str" cm="1">
-        <f t="array" ref="L97">INDEX(K$6:K$107,ROWS(K97:K$107))</f>
-        <v>&lt;td&gt;Final 17-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q15, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
     </row>
     <row r="98" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K98" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O36, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1.Wesley College &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L98" t="str" cm="1">
-        <f t="array" ref="L98">INDEX(K$6:K$107,ROWS(K98:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
       </c>
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
     </row>
     <row r="99" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K99" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P34, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Massey High School 2016 &lt;/td&gt;</v>
-      </c>
-      <c r="L99" t="str" cm="1">
-        <f t="array" ref="L99">INDEX(K$6:K$107,ROWS(K99:K$107))</f>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P15, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M99" s="10"/>
@@ -5967,235 +5380,251 @@
     </row>
     <row r="100" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K100" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P35, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final &lt;/td&gt;</v>
-      </c>
-      <c r="L100" t="str" cm="1">
-        <f t="array" ref="L100">INDEX(K$6:K$107,ROWS(K100:K$107))</f>
-        <v>&lt;td&gt;Final 12-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O13, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
       </c>
     </row>
     <row r="101" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K101" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", P36, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1.Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L101" t="str" cm="1">
-        <f t="array" ref="L101">INDEX(K$6:K$107,ROWS(K101:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O15, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="102" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K102" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q34, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Wellington 2017 &lt;/td&gt;</v>
-      </c>
-      <c r="L102" t="str" cm="1">
-        <f t="array" ref="L102">INDEX(K$6:K$107,ROWS(K102:K$107))</f>
-        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
       </c>
     </row>
     <row r="103" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K103" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q35, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 22-18 &lt;/td&gt;</v>
-      </c>
-      <c r="L103" t="str" cm="1">
-        <f t="array" ref="L103">INDEX(K$6:K$107,ROWS(K103:K$107))</f>
-        <v>&lt;td&gt;Final 8-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M103" s="10"/>
       <c r="N103" s="10"/>
     </row>
     <row r="104" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K104" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", Q36, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Christchurch BHS &lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L104" t="str" cm="1">
-        <f t="array" ref="L104">INDEX(K$6:K$107,ROWS(K104:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Napier 1986 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
       </c>
       <c r="M104" s="10"/>
       <c r="N104" s="10"/>
     </row>
     <row r="105" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K105" t="str">
-        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O37, "&lt;/td&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;Auckland Grammar 2018&lt;/td&gt;</v>
-      </c>
-      <c r="L105" t="str" cm="1">
-        <f t="array" ref="L105">INDEX(K$6:K$107,ROWS(K105:K$107))</f>
-        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", P12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M105" s="10"/>
       <c r="N105" s="10"/>
     </row>
     <row r="106" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K106" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O38, "&lt;/td&gt;")</f>
-        <v>&lt;td&gt;Final 17-21&lt;/td&gt;</v>
-      </c>
-      <c r="L106" t="str" cm="1">
-        <f t="array" ref="L106">INDEX(K$6:K$107,ROWS(K106:K$107))</f>
-        <v>&lt;td&gt;Final 14-3 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O10, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
       </c>
       <c r="M106" s="10"/>
       <c r="N106" s="10"/>
     </row>
     <row r="107" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K107" t="str">
-        <f>_xlfn.CONCAT("&lt;td&gt;", O39, "&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;td&gt;1. Hamilton BHS&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="L107" t="str" cm="1">
-        <f t="array" ref="L107">INDEX(K$6:K$107,ROWS(K107:K$107))</f>
-        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1985 &lt;/td&gt;</v>
+        <f>_xlfn.CONCAT("&lt;td&gt;", O12, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="M107" s="10"/>
       <c r="N107" s="10"/>
     </row>
     <row r="108" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K108" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
+      </c>
       <c r="L108" s="10"/>
       <c r="M108" s="10"/>
       <c r="N108" s="10"/>
     </row>
     <row r="109" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K109" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
       <c r="L109" s="10"/>
       <c r="M109" s="10"/>
       <c r="N109" s="10"/>
     </row>
     <row r="110" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K110" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
+      </c>
       <c r="L110" s="10"/>
       <c r="M110" s="10"/>
       <c r="N110" s="10"/>
     </row>
     <row r="111" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K111" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
       <c r="L111" s="10"/>
       <c r="M111" s="10"/>
       <c r="N111" s="10"/>
     </row>
     <row r="112" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K112" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O7, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>
+      </c>
       <c r="L112" s="10"/>
       <c r="M112" s="10"/>
       <c r="N112" s="10"/>
     </row>
-    <row r="113" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K113" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O9, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
       <c r="L113" s="10"/>
       <c r="M113" s="10"/>
       <c r="N113" s="10"/>
     </row>
-    <row r="114" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K114" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Auckland 1987 &lt;/td&gt;</v>
+      </c>
       <c r="L114" s="10"/>
       <c r="M114" s="10"/>
       <c r="N114" s="10"/>
     </row>
-    <row r="115" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K115" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", Q6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
       <c r="L115" s="10"/>
       <c r="M115" s="10"/>
       <c r="N115" s="10"/>
     </row>
-    <row r="116" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K116" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Napier 1986 &lt;/td&gt;</v>
+      </c>
       <c r="L116" s="10"/>
       <c r="M116" s="10"/>
       <c r="N116" s="10"/>
     </row>
-    <row r="117" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K117" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", P6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
       <c r="L117" s="10"/>
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
     </row>
-    <row r="118" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K118" t="str">
+        <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O4, "&lt;/td&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;Christchurch 1985 &lt;/td&gt;</v>
+      </c>
       <c r="L118" s="11"/>
       <c r="M118" s="11"/>
       <c r="N118" s="10"/>
     </row>
-    <row r="119" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="M119" s="13"/>
-      <c r="N119" s="13"/>
-    </row>
-    <row r="120" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="M120" s="13"/>
-      <c r="N120" s="13"/>
-    </row>
-    <row r="121" spans="12:14" x14ac:dyDescent="0.25">
-      <c r="M121" s="13"/>
-      <c r="N121" s="13"/>
-    </row>
-    <row r="122" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K119" t="str">
+        <f>_xlfn.CONCAT("&lt;td&gt;", O6, "&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="M119" s="36"/>
+      <c r="N119" s="36"/>
+    </row>
+    <row r="120" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="M120" s="36"/>
+      <c r="N120" s="36"/>
+    </row>
+    <row r="121" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="M121" s="36"/>
+      <c r="N121" s="36"/>
+    </row>
+    <row r="122" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L122" s="10"/>
-      <c r="M122" s="13"/>
-      <c r="N122" s="13"/>
-    </row>
-    <row r="123" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M122" s="36"/>
+      <c r="N122" s="36"/>
+    </row>
+    <row r="123" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L123" s="10"/>
-      <c r="M123" s="13"/>
-      <c r="N123" s="13"/>
-    </row>
-    <row r="124" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M123" s="36"/>
+      <c r="N123" s="36"/>
+    </row>
+    <row r="124" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L124" s="10"/>
-      <c r="M124" s="13"/>
-      <c r="N124" s="13"/>
-    </row>
-    <row r="125" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M124" s="36"/>
+      <c r="N124" s="36"/>
+    </row>
+    <row r="125" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L125" s="10"/>
-      <c r="M125" s="13"/>
-      <c r="N125" s="13"/>
-    </row>
-    <row r="126" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M125" s="36"/>
+      <c r="N125" s="36"/>
+    </row>
+    <row r="126" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L126" s="10"/>
-      <c r="M126" s="13"/>
-      <c r="N126" s="13"/>
-    </row>
-    <row r="127" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M126" s="36"/>
+      <c r="N126" s="36"/>
+    </row>
+    <row r="127" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L127" s="10"/>
-      <c r="M127" s="13"/>
-      <c r="N127" s="13"/>
-    </row>
-    <row r="128" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M127" s="36"/>
+      <c r="N127" s="36"/>
+    </row>
+    <row r="128" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L128" s="10"/>
-      <c r="M128" s="13"/>
-      <c r="N128" s="13"/>
+      <c r="M128" s="36"/>
+      <c r="N128" s="36"/>
     </row>
     <row r="129" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L129" s="10"/>
-      <c r="M129" s="13"/>
-      <c r="N129" s="13"/>
+      <c r="M129" s="36"/>
+      <c r="N129" s="36"/>
     </row>
     <row r="130" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L130" s="10"/>
-      <c r="M130" s="13"/>
-      <c r="N130" s="13"/>
+      <c r="M130" s="36"/>
+      <c r="N130" s="36"/>
     </row>
     <row r="131" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L131" s="10"/>
-      <c r="M131" s="13"/>
-      <c r="N131" s="13"/>
+      <c r="M131" s="36"/>
+      <c r="N131" s="36"/>
     </row>
     <row r="132" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L132" s="10"/>
-      <c r="M132" s="13"/>
-      <c r="N132" s="13"/>
+      <c r="M132" s="36"/>
+      <c r="N132" s="36"/>
     </row>
     <row r="133" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L133" s="10"/>
-      <c r="M133" s="13"/>
-      <c r="N133" s="13"/>
+      <c r="M133" s="36"/>
+      <c r="N133" s="36"/>
     </row>
     <row r="134" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L134" s="10"/>
-      <c r="M134" s="13"/>
-      <c r="N134" s="13"/>
+      <c r="M134" s="36"/>
+      <c r="N134" s="36"/>
     </row>
     <row r="135" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L135" s="10"/>
-      <c r="M135" s="13"/>
-      <c r="N135" s="13"/>
+      <c r="M135" s="36"/>
+      <c r="N135" s="36"/>
     </row>
     <row r="136" spans="12:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L136" s="10"/>
-      <c r="M136" s="13"/>
-      <c r="N136" s="13"/>
+      <c r="M136" s="36"/>
+      <c r="N136" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
adding results table and update time stamp
Signed-off-by: YelloElefant <alextrotternz@gmail.com>
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\13IA\Project\13IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FC1D6-A3EB-4960-94DC-D9EF11929F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{281FC1D6-A3EB-4960-94DC-D9EF11929F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F5A093C-1F85-45A0-8575-E78880F2E635}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
+    <workbookView xWindow="-22320" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{F888C5C3-F0AE-438E-8393-F3BEF9854CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="194">
   <si>
     <r>
       <t>&lt;</t>
@@ -3127,13 +3127,52 @@
   </si>
   <si>
     <t>UNI 2</t>
+  </si>
+  <si>
+    <t>Rotorua Boys' HS</t>
+  </si>
+  <si>
+    <t>New Plymouth Boys; HS</t>
+  </si>
+  <si>
+    <t>Hamilton Boys' HS</t>
+  </si>
+  <si>
+    <t>Hastings Boys' HS</t>
+  </si>
+  <si>
+    <t>Auckland Grammar</t>
+  </si>
+  <si>
+    <t>Palmerston North Boys' HS</t>
+  </si>
+  <si>
+    <t>Christchurch Boys' HS</t>
+  </si>
+  <si>
+    <t>Napier Boys' HS</t>
+  </si>
+  <si>
+    <t>St Pats College</t>
+  </si>
+  <si>
+    <t>Westlake Boys' HS</t>
+  </si>
+  <si>
+    <t>Mount Albert GS</t>
+  </si>
+  <si>
+    <t>St Bedes College</t>
+  </si>
+  <si>
+    <t>Otago Boys' HS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3201,6 +3240,12 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3216,7 +3261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -3447,11 +3492,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3548,6 +3608,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3865,14 +3928,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD87F2E1-A52F-4456-AB4D-EECF95DE5FBF}">
   <dimension ref="B3:Y136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52:K119"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
     <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="43.42578125" bestFit="1" customWidth="1"/>
@@ -5250,7 +5314,7 @@
         <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="84" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K84" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q19, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Palmerston North 2002 &lt;/td&gt;</v>
@@ -5258,7 +5322,14 @@
       <c r="M84" s="10"/>
       <c r="N84" s="10"/>
     </row>
-    <row r="85" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F85" t="str">
+        <f>CONCATENATE("&lt;div class='card'&gt;",E85,"&lt;/div&gt;")</f>
+        <v>&lt;div class='card'&gt;Rotorua Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K85" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q21, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Napier BHS &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5266,7 +5337,14 @@
       <c r="M85" s="10"/>
       <c r="N85" s="10"/>
     </row>
-    <row r="86" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" ref="F86:F101" si="12">CONCATENATE("&lt;div class='card'&gt;",E86,"&lt;/div&gt;")</f>
+        <v>&lt;div class='card'&gt;Wellington College&lt;/div&gt;</v>
+      </c>
       <c r="K86" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P19, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Dunedin 2001 &lt;/td&gt;</v>
@@ -5274,7 +5352,14 @@
       <c r="M86" s="10"/>
       <c r="N86" s="10"/>
     </row>
-    <row r="87" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="F87" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Tauranga Boys College&lt;/div&gt;</v>
+      </c>
       <c r="K87" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", P21, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar School &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5282,7 +5367,14 @@
       <c r="M87" s="10"/>
       <c r="N87" s="10"/>
     </row>
-    <row r="88" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E88" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;New Plymouth Boys; HS&lt;/div&gt;</v>
+      </c>
       <c r="K88" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O19, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Wellington 2000 &lt;/td&gt;</v>
@@ -5290,7 +5382,14 @@
       <c r="M88" s="10"/>
       <c r="N88" s="10"/>
     </row>
-    <row r="89" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="F89" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Hamilton Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K89" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", O21, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Hastings BHS &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5298,7 +5397,14 @@
       <c r="M89" s="10"/>
       <c r="N89" s="10"/>
     </row>
-    <row r="90" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="F90" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Hastings Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K90" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q16, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Auckland 1999 &lt;/td&gt;</v>
@@ -5306,7 +5412,14 @@
       <c r="M90" s="10"/>
       <c r="N90" s="10"/>
     </row>
-    <row r="91" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="F91" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Auckland Grammar&lt;/div&gt;</v>
+      </c>
       <c r="K91" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q18, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Otago BHS &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5314,7 +5427,14 @@
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
     </row>
-    <row r="92" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="F92" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Palmerston North Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K92" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P16, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Napier 1998 &lt;/td&gt;</v>
@@ -5322,7 +5442,14 @@
       <c r="M92" s="10"/>
       <c r="N92" s="10"/>
     </row>
-    <row r="93" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E93" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F93" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Christchurch Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K93" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", P18, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5330,7 +5457,14 @@
       <c r="M93" s="10"/>
       <c r="N93" s="10"/>
     </row>
-    <row r="94" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E94" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F94" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Napier Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K94" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O16, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Christchurch 1997 &lt;/td&gt;</v>
@@ -5338,7 +5472,14 @@
       <c r="M94" s="10"/>
       <c r="N94" s="10"/>
     </row>
-    <row r="95" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="F95" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;St Pats College&lt;/div&gt;</v>
+      </c>
       <c r="K95" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", O18, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5346,7 +5487,14 @@
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
     </row>
-    <row r="96" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E96" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="F96" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Westlake Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K96" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q13, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Hamilton 1996 &lt;/td&gt;</v>
@@ -5354,7 +5502,14 @@
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
     </row>
-    <row r="97" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Mount Albert GS&lt;/div&gt;</v>
+      </c>
       <c r="K97" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q15, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5362,7 +5517,14 @@
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
     </row>
-    <row r="98" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E98" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;St Bedes College&lt;/div&gt;</v>
+      </c>
       <c r="K98" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P13, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Dunedin 1995 &lt;/td&gt;</v>
@@ -5370,7 +5532,14 @@
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
     </row>
-    <row r="99" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Wesley College&lt;/div&gt;</v>
+      </c>
       <c r="K99" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", P15, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5378,25 +5547,36 @@
       <c r="M99" s="10"/>
       <c r="N99" s="10"/>
     </row>
-    <row r="100" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E100" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;Otago Boys' HS&lt;/div&gt;</v>
+      </c>
       <c r="K100" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O13, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Wellington 1994 &lt;/td&gt;</v>
       </c>
     </row>
-    <row r="101" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="F101" t="str">
+        <f t="shared" si="12"/>
+        <v>&lt;div class='card'&gt;&lt;/div&gt;</v>
+      </c>
       <c r="K101" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", O15, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="102" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:14" x14ac:dyDescent="0.25">
       <c r="K102" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q10, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Auckland 1993 &lt;/td&gt;</v>
       </c>
     </row>
-    <row r="103" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K103" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q12, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5404,7 +5584,7 @@
       <c r="M103" s="10"/>
       <c r="N103" s="10"/>
     </row>
-    <row r="104" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K104" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P10, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Napier 1992 &lt;/td&gt;</v>
@@ -5412,7 +5592,7 @@
       <c r="M104" s="10"/>
       <c r="N104" s="10"/>
     </row>
-    <row r="105" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K105" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", P12, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Mt Albert Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5420,7 +5600,7 @@
       <c r="M105" s="10"/>
       <c r="N105" s="10"/>
     </row>
-    <row r="106" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K106" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O10, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Christchurch 1991 &lt;/td&gt;</v>
@@ -5428,7 +5608,7 @@
       <c r="M106" s="10"/>
       <c r="N106" s="10"/>
     </row>
-    <row r="107" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K107" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", O12, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. Auckland Grammar &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5436,7 +5616,7 @@
       <c r="M107" s="10"/>
       <c r="N107" s="10"/>
     </row>
-    <row r="108" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K108" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", Q7, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Hamilton 1990 &lt;/td&gt;</v>
@@ -5445,7 +5625,7 @@
       <c r="M108" s="10"/>
       <c r="N108" s="10"/>
     </row>
-    <row r="109" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K109" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", Q9, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5454,7 +5634,7 @@
       <c r="M109" s="10"/>
       <c r="N109" s="10"/>
     </row>
-    <row r="110" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K110" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", P7, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Dunedin 1989 &lt;/td&gt;</v>
@@ -5463,7 +5643,7 @@
       <c r="M110" s="10"/>
       <c r="N110" s="10"/>
     </row>
-    <row r="111" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K111" t="str">
         <f>_xlfn.CONCAT("&lt;td&gt;", P9, "&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;td&gt;1. St Stephen’s School &lt;/td&gt;&lt;/tr&gt;</v>
@@ -5472,7 +5652,7 @@
       <c r="M111" s="10"/>
       <c r="N111" s="10"/>
     </row>
-    <row r="112" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K112" t="str">
         <f>_xlfn.CONCAT("&lt;tr&gt;&lt;td&gt;", O7, "&lt;/td&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Wellington 1988 &lt;/td&gt;</v>

</xml_diff>